<commit_message>
+* BGU-105 WPF XAML генератор (зі структур) : in progress (concrete steps): fixed binding errors, added diagnostics, etc.
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9915" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9915" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="302">
   <si>
     <t>ClassName</t>
   </si>
@@ -1251,7 +1251,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1915,7 +1915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C53" workbookViewId="0">
+    <sheetView topLeftCell="C53" workbookViewId="0">
       <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
@@ -6096,7 +6096,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7090,9 +7090,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:E32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7142,7 +7144,7 @@
         <v>250</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B30" si="0">"List"&amp;TRIM(A3)</f>
+        <f t="shared" ref="B3:B32" si="0">"List"&amp;TRIM(A3)</f>
         <v>ListOwnershipType</v>
       </c>
       <c r="C3" t="str">
@@ -7150,11 +7152,11 @@
         <v>public List&lt;EnumType&gt; ListOwnershipType() { return EnumType.GetEnumList(typeof(OwnershipType)); }</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D30" si="2">A3&amp;"List"</f>
+        <f t="shared" ref="D3:D32" si="2">A3&amp;"List"</f>
         <v>OwnershipTypeList</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E30" si="3">"public static List&lt;EnumType&gt; "&amp;D3 &amp;" { get { return EnumType.GetEnumList(typeof("&amp;A3&amp;")); }}"</f>
+        <f t="shared" ref="E3:E32" si="3">"public static List&lt;EnumType&gt; "&amp;D3 &amp;" { get { return EnumType.GetEnumList(typeof("&amp;A3&amp;")); }}"</f>
         <v>public static List&lt;EnumType&gt; OwnershipTypeList { get { return EnumType.GetEnumList(typeof(OwnershipType)); }}</v>
       </c>
     </row>
@@ -7650,7 +7652,7 @@
         <v>ListFinancialInstitutionType</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" ref="C27:C30" si="4">"public List&lt;EnumType&gt; "&amp;B27 &amp;"() { return EnumType.GetEnumList(typeof("&amp;A27&amp;")); }"</f>
+        <f t="shared" ref="C27:C32" si="4">"public List&lt;EnumType&gt; "&amp;B27 &amp;"() { return EnumType.GetEnumList(typeof("&amp;A27&amp;")); }"</f>
         <v>public List&lt;EnumType&gt; ListFinancialInstitutionType() { return EnumType.GetEnumList(typeof(FinancialInstitutionType)); }</v>
       </c>
       <c r="D27" t="str">
@@ -7723,6 +7725,48 @@
       <c r="E30" t="str">
         <f t="shared" si="3"/>
         <v>public static List&lt;EnumType&gt; InstitutionLevelList { get { return EnumType.GetEnumList(typeof(InstitutionLevel)); }}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>283</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>ListLegalTransactionType</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="4"/>
+        <v>public List&lt;EnumType&gt; ListLegalTransactionType() { return EnumType.GetEnumList(typeof(LegalTransactionType)); }</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>LegalTransactionTypeList</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="3"/>
+        <v>public static List&lt;EnumType&gt; LegalTransactionTypeList { get { return EnumType.GetEnumList(typeof(LegalTransactionType)); }}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>284</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>ListInfluenceType</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="4"/>
+        <v>public List&lt;EnumType&gt; ListInfluenceType() { return EnumType.GetEnumList(typeof(InfluenceType)); }</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>InfluenceTypeList</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="3"/>
+        <v>public static List&lt;EnumType&gt; InfluenceTypeList { get { return EnumType.GetEnumList(typeof(InfluenceType)); }}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+* BGU-105 WPF XAML генератор (зі структур) : in progress (concrete steps): fighting further
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9915" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9915" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="XSDTypeTransls" sheetId="4" r:id="rId4"/>
     <sheet name="Enums" sheetId="5" r:id="rId5"/>
     <sheet name="EnumsLister" sheetId="6" r:id="rId6"/>
+    <sheet name="WPF_temp_test" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="306">
   <si>
     <t>ClassName</t>
   </si>
@@ -930,6 +931,18 @@
   </si>
   <si>
     <t>PowerOfAttorneyInfo</t>
+  </si>
+  <si>
+    <t>MissingInformationResonInfo</t>
+  </si>
+  <si>
+    <t>TypeName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quCtrl.Content = new </t>
+  </si>
+  <si>
+    <t>(); MessageBox.Show("Press OK to continue...");</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1264,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7092,7 +7105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31:E32"/>
     </sheetView>
   </sheetViews>
@@ -7773,4 +7786,417 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="str">
+        <f>$B$1&amp;A2&amp;$C$1</f>
+        <v>quCtrl.Content = new BankInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B44" si="0">$B$1&amp;A3&amp;$C$1</f>
+        <v>quCtrl.Content = new BankruptcyInvestigationInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new BreachOfLawRecordInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new ContactInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new CountryInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new CourtDecisionInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new CourtInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new CreditRatingInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new CurrencyAmount(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new EconomicActivityType(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new EmailInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new FinancialOversightAuthorityInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new GenericPersonID(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new GenericPersonInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new ImperfectBusinessReputationInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new IncomeOriginInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new IndebtnessInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new IPOSharesPurchaseInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new LegalPersonInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new LegalTransactionInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new LiquidatedEntityOwnershipInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new LoanInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new LocationInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new LPRegisteredDateRecordId(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>302</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new MissingInformationResonInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new OwnershipStructure(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new OwnershipSummaryInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new OwnershipVotesInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new PaymentDeadlineInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new PersonsAssociation(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new PhoneInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new PhysicalPersonInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>301</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new PowerOfAttorneyInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>296</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new PowerOfAttorneySharesPurchaseInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>288</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new RatingAgencyInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new RegistrarAuthority(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new RegLicAppx2OwnershipAcqRequestLP(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new SecondaryMarketSharesPurchaseInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new SignatoryInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>297</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new SignificantOrDecisiveInfulenceInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>298</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new SignificantOwnershipAcquisitionWaysInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new TotalOwnershipDetailsInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>299</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>quCtrl.Content = new TotalOwnershipSummaryInfo(); MessageBox.Show("Press OK to continue...");</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+ BGUSO-93 WPFGen: Apply conditional visibility : In progress
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9915" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9915" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Enums" sheetId="5" r:id="rId5"/>
     <sheet name="EnumsLister" sheetId="6" r:id="rId6"/>
     <sheet name="WPF_temp_test" sheetId="7" r:id="rId7"/>
+    <sheet name="NotifyPropertyChanged" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="318">
   <si>
     <t>ClassName</t>
   </si>
@@ -943,6 +944,42 @@
   </si>
   <si>
     <t>(); MessageBox.Show("Press OK to continue...");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public string NameUkr { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public CountryInfo JurisdictionCountry { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public string CourtRegion { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public string CourtID { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public CourtInstanceType Instance { get; set; }</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Modifier</t>
+  </si>
+  <si>
+    <t>PropName</t>
+  </si>
+  <si>
+    <t>FieldName</t>
+  </si>
+  <si>
+    <t>FieldDecl</t>
+  </si>
+  <si>
+    <t>Accessor</t>
+  </si>
+  <si>
+    <t>public string ShortTermRatingValueOther { get; set; }</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7792,7 +7829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B44"/>
     </sheetView>
   </sheetViews>
@@ -8199,4 +8236,332 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="10" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" t="str">
+        <f>TRIM(A2)</f>
+        <v>public string ShortTermRatingValueOther { get; set; }</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>FIND(" ",$B2)</f>
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <f>FIND(" ",$B2,D2+1)</f>
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <f>FIND(" ",$B2,E2+1)</f>
+        <v>40</v>
+      </c>
+      <c r="G2" t="str">
+        <f>TRIM(MID($B2,C2,D2-C2))</f>
+        <v>public</v>
+      </c>
+      <c r="H2" t="str">
+        <f>TRIM(MID($B2,D2,E2-D2))</f>
+        <v>string</v>
+      </c>
+      <c r="I2" t="str">
+        <f>TRIM(MID($B2,E2,F2-E2))</f>
+        <v>ShortTermRatingValueOther</v>
+      </c>
+      <c r="J2" t="str">
+        <f>"_"&amp;I2</f>
+        <v>_ShortTermRatingValueOther</v>
+      </c>
+      <c r="K2" t="str">
+        <f>"private " &amp; H2 &amp; " " &amp; J2 &amp; ";"</f>
+        <v>private string _ShortTermRatingValueOther;</v>
+      </c>
+      <c r="L2" t="str">
+        <f>G2&amp; " " &amp;H2&amp; " " &amp;I2 &amp; " { get { return " &amp; J2 &amp; "; } set { " &amp;J2 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I2 &amp; CHAR(34) &amp; "); } }"</f>
+        <v>public string ShortTermRatingValueOther { get { return _ShortTermRatingValueOther; } set { _ShortTermRatingValueOther = value; OnPropertyChanged("ShortTermRatingValueOther"); } }</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B7" si="0">TRIM(A3)</f>
+        <v>public string NameUkr { get; set; }</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="1">FIND(" ",$B3)</f>
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:F7" si="2">FIND(" ",$B3,D3+1)</f>
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G7" si="3">TRIM(MID($B3,C3,D3-C3))</f>
+        <v>public</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H7" si="4">TRIM(MID($B3,D3,E3-D3))</f>
+        <v>string</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I7" si="5">TRIM(MID($B3,E3,F3-E3))</f>
+        <v>NameUkr</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J7" si="6">"_"&amp;I3</f>
+        <v>_NameUkr</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K7" si="7">"private " &amp; H3 &amp; " " &amp; J3 &amp; ";"</f>
+        <v>private string _NameUkr;</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L7" si="8">G3&amp; " " &amp;H3&amp; " " &amp;I3 &amp; " { get { return " &amp; J3 &amp; "; } set { " &amp;J3 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I3 &amp; CHAR(34) &amp; "); } }"</f>
+        <v>public string NameUkr { get { return _NameUkr; } set { _NameUkr = value; OnPropertyChanged("NameUkr"); } }</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>public CountryInfo JurisdictionCountry { get; set; }</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="3"/>
+        <v>public</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="4"/>
+        <v>CountryInfo</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="5"/>
+        <v>JurisdictionCountry</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="6"/>
+        <v>_JurisdictionCountry</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="7"/>
+        <v>private CountryInfo _JurisdictionCountry;</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="8"/>
+        <v>public CountryInfo JurisdictionCountry { get { return _JurisdictionCountry; } set { _JurisdictionCountry = value; OnPropertyChanged("JurisdictionCountry"); } }</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>public string CourtRegion { get; set; }</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="3"/>
+        <v>public</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="4"/>
+        <v>string</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="5"/>
+        <v>CourtRegion</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="6"/>
+        <v>_CourtRegion</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="7"/>
+        <v>private string _CourtRegion;</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="8"/>
+        <v>public string CourtRegion { get { return _CourtRegion; } set { _CourtRegion = value; OnPropertyChanged("CourtRegion"); } }</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>public string CourtID { get; set; }</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="3"/>
+        <v>public</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="4"/>
+        <v>string</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="5"/>
+        <v>CourtID</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="6"/>
+        <v>_CourtID</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="7"/>
+        <v>private string _CourtID;</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="8"/>
+        <v>public string CourtID { get { return _CourtID; } set { _CourtID = value; OnPropertyChanged("CourtID"); } }</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>public CourtInstanceType Instance { get; set; }</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>public</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>CourtInstanceType</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="5"/>
+        <v>Instance</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v>_Instance</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="7"/>
+        <v>private CourtInstanceType _Instance;</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="8"/>
+        <v>public CourtInstanceType Instance { get { return _Instance; } set { _Instance = value; OnPropertyChanged("Instance"); } }</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+ BGUSO-93 WPFGen: Apply conditional visibility : largely done, enough so far
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -979,7 +979,7 @@
     <t>Accessor</t>
   </si>
   <si>
-    <t>public string ShortTermRatingValueOther { get; set; }</t>
+    <t>public bool IsIPNRefused { get; set; }</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8278,7 +8278,7 @@
       </c>
       <c r="B2" t="str">
         <f>TRIM(A2)</f>
-        <v>public string ShortTermRatingValueOther { get; set; }</v>
+        <v>public bool IsIPNRefused { get; set; }</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8289,11 +8289,11 @@
       </c>
       <c r="E2">
         <f>FIND(" ",$B2,D2+1)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <f>FIND(" ",$B2,E2+1)</f>
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G2" t="str">
         <f>TRIM(MID($B2,C2,D2-C2))</f>
@@ -8301,23 +8301,23 @@
       </c>
       <c r="H2" t="str">
         <f>TRIM(MID($B2,D2,E2-D2))</f>
-        <v>string</v>
+        <v>bool</v>
       </c>
       <c r="I2" t="str">
         <f>TRIM(MID($B2,E2,F2-E2))</f>
-        <v>ShortTermRatingValueOther</v>
+        <v>IsIPNRefused</v>
       </c>
       <c r="J2" t="str">
         <f>"_"&amp;I2</f>
-        <v>_ShortTermRatingValueOther</v>
+        <v>_IsIPNRefused</v>
       </c>
       <c r="K2" t="str">
         <f>"private " &amp; H2 &amp; " " &amp; J2 &amp; ";"</f>
-        <v>private string _ShortTermRatingValueOther;</v>
+        <v>private bool _IsIPNRefused;</v>
       </c>
       <c r="L2" t="str">
         <f>G2&amp; " " &amp;H2&amp; " " &amp;I2 &amp; " { get { return " &amp; J2 &amp; "; } set { " &amp;J2 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I2 &amp; CHAR(34) &amp; "); } }"</f>
-        <v>public string ShortTermRatingValueOther { get { return _ShortTermRatingValueOther; } set { _ShortTermRatingValueOther = value; OnPropertyChanged("ShortTermRatingValueOther"); } }</v>
+        <v>public bool IsIPNRefused { get { return _IsIPNRefused; } set { _IsIPNRefused = value; OnPropertyChanged("IsIPNRefused"); } }</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+* BGUSO-94 WPFGen: Do something about data grids' look and feel : in progress
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -979,7 +979,7 @@
     <t>Accessor</t>
   </si>
   <si>
-    <t>public bool IsIPNRefused { get; set; }</t>
+    <t>public ContactInfo ContactPerson { get; set; }</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8278,7 +8278,7 @@
       </c>
       <c r="B2" t="str">
         <f>TRIM(A2)</f>
-        <v>public bool IsIPNRefused { get; set; }</v>
+        <v>public ContactInfo ContactPerson { get; set; }</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8289,11 +8289,11 @@
       </c>
       <c r="E2">
         <f>FIND(" ",$B2,D2+1)</f>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <f>FIND(" ",$B2,E2+1)</f>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G2" t="str">
         <f>TRIM(MID($B2,C2,D2-C2))</f>
@@ -8301,23 +8301,23 @@
       </c>
       <c r="H2" t="str">
         <f>TRIM(MID($B2,D2,E2-D2))</f>
-        <v>bool</v>
+        <v>ContactInfo</v>
       </c>
       <c r="I2" t="str">
         <f>TRIM(MID($B2,E2,F2-E2))</f>
-        <v>IsIPNRefused</v>
+        <v>ContactPerson</v>
       </c>
       <c r="J2" t="str">
         <f>"_"&amp;I2</f>
-        <v>_IsIPNRefused</v>
+        <v>_ContactPerson</v>
       </c>
       <c r="K2" t="str">
         <f>"private " &amp; H2 &amp; " " &amp; J2 &amp; ";"</f>
-        <v>private bool _IsIPNRefused;</v>
+        <v>private ContactInfo _ContactPerson;</v>
       </c>
       <c r="L2" t="str">
         <f>G2&amp; " " &amp;H2&amp; " " &amp;I2 &amp; " { get { return " &amp; J2 &amp; "; } set { " &amp;J2 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I2 &amp; CHAR(34) &amp; "); } }"</f>
-        <v>public bool IsIPNRefused { get { return _IsIPNRefused; } set { _IsIPNRefused = value; OnPropertyChanged("IsIPNRefused"); } }</v>
+        <v>public ContactInfo ContactPerson { get { return _ContactPerson; } set { _ContactPerson = value; OnPropertyChanged("ContactPerson"); } }</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+* BGUSO-15 WPF XAML генератор (зі структур) : finishing touches
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -979,7 +979,7 @@
     <t>Accessor</t>
   </si>
   <si>
-    <t>public ContactInfo ContactPerson { get; set; }</t>
+    <t>public string RepaymentPlans { get; set; }</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8278,7 +8278,7 @@
       </c>
       <c r="B2" t="str">
         <f>TRIM(A2)</f>
-        <v>public ContactInfo ContactPerson { get; set; }</v>
+        <v>public string RepaymentPlans { get; set; }</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8289,11 +8289,11 @@
       </c>
       <c r="E2">
         <f>FIND(" ",$B2,D2+1)</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <f>FIND(" ",$B2,E2+1)</f>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G2" t="str">
         <f>TRIM(MID($B2,C2,D2-C2))</f>
@@ -8301,23 +8301,23 @@
       </c>
       <c r="H2" t="str">
         <f>TRIM(MID($B2,D2,E2-D2))</f>
-        <v>ContactInfo</v>
+        <v>string</v>
       </c>
       <c r="I2" t="str">
         <f>TRIM(MID($B2,E2,F2-E2))</f>
-        <v>ContactPerson</v>
+        <v>RepaymentPlans</v>
       </c>
       <c r="J2" t="str">
         <f>"_"&amp;I2</f>
-        <v>_ContactPerson</v>
+        <v>_RepaymentPlans</v>
       </c>
       <c r="K2" t="str">
         <f>"private " &amp; H2 &amp; " " &amp; J2 &amp; ";"</f>
-        <v>private ContactInfo _ContactPerson;</v>
+        <v>private string _RepaymentPlans;</v>
       </c>
       <c r="L2" t="str">
         <f>G2&amp; " " &amp;H2&amp; " " &amp;I2 &amp; " { get { return " &amp; J2 &amp; "; } set { " &amp;J2 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I2 &amp; CHAR(34) &amp; "); } }"</f>
-        <v>public ContactInfo ContactPerson { get { return _ContactPerson; } set { _ContactPerson = value; OnPropertyChanged("ContactPerson"); } }</v>
+        <v>public string RepaymentPlans { get { return _RepaymentPlans; } set { _RepaymentPlans = value; OnPropertyChanged("RepaymentPlans"); } }</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+ BGUSO-108 WPFGen: Miscellaneous finishing touches : In progress
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -946,9 +946,6 @@
     <t>(); MessageBox.Show("Press OK to continue...");</t>
   </si>
   <si>
-    <t xml:space="preserve">        public string NameUkr { get; set; }</t>
-  </si>
-  <si>
     <t xml:space="preserve">        public CountryInfo JurisdictionCountry { get; set; }</t>
   </si>
   <si>
@@ -979,7 +976,10 @@
     <t>Accessor</t>
   </si>
   <si>
-    <t>public string RepaymentPlans { get; set; }</t>
+    <t xml:space="preserve">        public string DecisionRegistryID { get; set; }</t>
+  </si>
+  <si>
+    <t>public string DecisionTextSummary { get; set; }</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8243,7 +8243,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K2" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8253,22 +8253,22 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="M1" s="1"/>
     </row>
@@ -8278,7 +8278,7 @@
       </c>
       <c r="B2" t="str">
         <f>TRIM(A2)</f>
-        <v>public string RepaymentPlans { get; set; }</v>
+        <v>public string DecisionTextSummary { get; set; }</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="F2">
         <f>FIND(" ",$B2,E2+1)</f>
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G2" t="str">
         <f>TRIM(MID($B2,C2,D2-C2))</f>
@@ -8305,28 +8305,28 @@
       </c>
       <c r="I2" t="str">
         <f>TRIM(MID($B2,E2,F2-E2))</f>
-        <v>RepaymentPlans</v>
+        <v>DecisionTextSummary</v>
       </c>
       <c r="J2" t="str">
         <f>"_"&amp;I2</f>
-        <v>_RepaymentPlans</v>
+        <v>_DecisionTextSummary</v>
       </c>
       <c r="K2" t="str">
         <f>"private " &amp; H2 &amp; " " &amp; J2 &amp; ";"</f>
-        <v>private string _RepaymentPlans;</v>
+        <v>private string _DecisionTextSummary;</v>
       </c>
       <c r="L2" t="str">
         <f>G2&amp; " " &amp;H2&amp; " " &amp;I2 &amp; " { get { return " &amp; J2 &amp; "; } set { " &amp;J2 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I2 &amp; CHAR(34) &amp; "); } }"</f>
-        <v>public string RepaymentPlans { get { return _RepaymentPlans; } set { _RepaymentPlans = value; OnPropertyChanged("RepaymentPlans"); } }</v>
+        <v>public string DecisionTextSummary { get { return _DecisionTextSummary; } set { _DecisionTextSummary = value; OnPropertyChanged("DecisionTextSummary"); } }</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B7" si="0">TRIM(A3)</f>
-        <v>public string NameUkr { get; set; }</v>
+        <v>public string DecisionRegistryID { get; set; }</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -8341,7 +8341,7 @@
       </c>
       <c r="F3">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" si="3">TRIM(MID($B3,C3,D3-C3))</f>
@@ -8353,24 +8353,24 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I7" si="5">TRIM(MID($B3,E3,F3-E3))</f>
-        <v>NameUkr</v>
+        <v>DecisionRegistryID</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J7" si="6">"_"&amp;I3</f>
-        <v>_NameUkr</v>
+        <v>_DecisionRegistryID</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K7" si="7">"private " &amp; H3 &amp; " " &amp; J3 &amp; ";"</f>
-        <v>private string _NameUkr;</v>
+        <v>private string _DecisionRegistryID;</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L7" si="8">G3&amp; " " &amp;H3&amp; " " &amp;I3 &amp; " { get { return " &amp; J3 &amp; "; } set { " &amp;J3 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I3 &amp; CHAR(34) &amp; "); } }"</f>
-        <v>public string NameUkr { get { return _NameUkr; } set { _NameUkr = value; OnPropertyChanged("NameUkr"); } }</v>
+        <v>public string DecisionRegistryID { get { return _DecisionRegistryID; } set { _DecisionRegistryID = value; OnPropertyChanged("DecisionRegistryID"); } }</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -8418,7 +8418,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -8466,7 +8466,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -8514,7 +8514,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
+ BGUSO-147 Sensitive data anonymizer - started
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -1219,13 +1219,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t xml:space="preserve">        public List&lt;EmploymentRecordInfo&gt; MgrWorkExperience { get; set; }</t>
-  </si>
-  <si>
     <t xml:space="preserve">        public PersonBusinessReputationInfo MgrBusinessReputation { get; set; }</t>
   </si>
   <si>
-    <t>public string MgrPositionOther { get; set; }</t>
+    <t xml:space="preserve">        public bool HasDoubleCitizenship { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public List&lt;CountryInfo&gt; DoubleCitizenshipCountries { get; set; }</t>
   </si>
 </sst>
 </file>
@@ -1545,7 +1545,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9182,7 +9182,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9214,11 +9214,11 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B7" si="0">TRIM(A2)</f>
-        <v>public string MgrPositionOther { get; set; }</v>
+        <v>public bool HasDoubleCitizenship { get; set; }</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -9229,11 +9229,11 @@
       </c>
       <c r="E2">
         <f>FIND(" ",$B2,D2+1)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <f>FIND(" ",$B2,E2+1)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:I7" si="2">TRIM(MID($B2,C2,D2-C2))</f>
@@ -9241,32 +9241,32 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" si="2"/>
-        <v>string</v>
+        <v>bool</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" si="2"/>
-        <v>MgrPositionOther</v>
+        <v>HasDoubleCitizenship</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J7" si="3">"_"&amp;I2</f>
-        <v>_MgrPositionOther</v>
+        <v>_HasDoubleCitizenship</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" ref="K2:K7" si="4">"private " &amp; H2 &amp; " " &amp; J2 &amp; ";"</f>
-        <v>private string _MgrPositionOther;</v>
+        <v>private bool _HasDoubleCitizenship;</v>
       </c>
       <c r="L2" t="str">
         <f t="shared" ref="L2:L15" si="5">G2&amp; " " &amp;H2&amp; " " &amp;I2 &amp; " { get { return " &amp; J2 &amp; "; } set { " &amp;J2 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I2 &amp; CHAR(34) &amp; "); } }"</f>
-        <v>public string MgrPositionOther { get { return _MgrPositionOther; } set { _MgrPositionOther = value; OnPropertyChanged("MgrPositionOther"); } }</v>
+        <v>public bool HasDoubleCitizenship { get { return _HasDoubleCitizenship; } set { _HasDoubleCitizenship = value; OnPropertyChanged("HasDoubleCitizenship"); } }</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>public List&lt;EmploymentRecordInfo&gt; MgrWorkExperience { get; set; }</v>
+        <v>public List&lt;CountryInfo&gt; DoubleCitizenshipCountries { get; set; }</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -9277,7 +9277,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:F7" si="6">FIND(" ",$B3,D3+1)</f>
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <f t="shared" si="6"/>
@@ -9289,28 +9289,28 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" si="2"/>
-        <v>List&lt;EmploymentRecordInfo&gt;</v>
+        <v>List&lt;CountryInfo&gt;</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="2"/>
-        <v>MgrWorkExperience</v>
+        <v>DoubleCitizenshipCountries</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="3"/>
-        <v>_MgrWorkExperience</v>
+        <v>_DoubleCitizenshipCountries</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="4"/>
-        <v>private List&lt;EmploymentRecordInfo&gt; _MgrWorkExperience;</v>
+        <v>private List&lt;CountryInfo&gt; _DoubleCitizenshipCountries;</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="5"/>
-        <v>public List&lt;EmploymentRecordInfo&gt; MgrWorkExperience { get { return _MgrWorkExperience; } set { _MgrWorkExperience = value; OnPropertyChanged("MgrWorkExperience"); } }</v>
+        <v>public List&lt;CountryInfo&gt; DoubleCitizenshipCountries { get { return _DoubleCitizenshipCountries; } set { _DoubleCitizenshipCountries = value; OnPropertyChanged("DoubleCitizenshipCountries"); } }</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
+* BKRGSTR-21 Ел.еквівалент додатку 15 - v.1 : In progress, largely done
</commit_message>
<xml_diff>
--- a/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
+++ b/SignOwn/CSharp/Codegen/BGU_xsd_outil16.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="610">
   <si>
     <t>ClassName</t>
   </si>
@@ -1800,6 +1800,60 @@
   </si>
   <si>
     <t>ApptOfficeNrOld</t>
+  </si>
+  <si>
+    <t>Oblast</t>
+  </si>
+  <si>
+    <t>IsOblastChanged</t>
+  </si>
+  <si>
+    <t>OblastNew</t>
+  </si>
+  <si>
+    <t>OblastOld</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>IsPhoneChanged</t>
+  </si>
+  <si>
+    <t>PhoneNew</t>
+  </si>
+  <si>
+    <t>PhoneOld</t>
+  </si>
+  <si>
+    <t>FinActivitySvcInstrumentActionType</t>
+  </si>
+  <si>
+    <t>FinActivitySvcInstrumentType</t>
+  </si>
+  <si>
+    <t>OperationsListing</t>
+  </si>
+  <si>
+    <t>IsOperationsListingChanged</t>
+  </si>
+  <si>
+    <t>OperationsListingNew</t>
+  </si>
+  <si>
+    <t>OperationsListingOld</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>IsStatusChanged</t>
+  </si>
+  <si>
+    <t>StatusNew</t>
+  </si>
+  <si>
+    <t>StatusOld</t>
   </si>
 </sst>
 </file>
@@ -2119,7 +2173,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2946,10 +3000,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:E33"/>
+      <selection activeCell="C37" sqref="C37:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2990,15 +3044,15 @@
         <v>462</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C33" si="0">"Is" &amp; B3 &amp;"Changed"</f>
+        <f t="shared" ref="C3:C35" si="0">"Is" &amp; B3 &amp;"Changed"</f>
         <v>IsNameFullChanged</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D27" si="1">B3&amp;"New"</f>
+        <f t="shared" ref="D3:D29" si="1">B3&amp;"New"</f>
         <v>NameFullNew</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E27" si="2">B3&amp;"Old"</f>
+        <f t="shared" ref="E3:E29" si="2">B3&amp;"Old"</f>
         <v>NameFullOld</v>
       </c>
     </row>
@@ -3227,19 +3281,19 @@
         <v>460</v>
       </c>
       <c r="B15" t="s">
-        <v>474</v>
+        <v>596</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>IsFaxChanged</v>
+        <v>IsPhoneChanged</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
-        <v>FaxNew</v>
+        <v>PhoneNew</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="2"/>
-        <v>FaxOld</v>
+        <v>PhoneOld</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3247,19 +3301,19 @@
         <v>460</v>
       </c>
       <c r="B16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>IsEmailChanged</v>
+        <v>IsFaxChanged</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
-        <v>EmailNew</v>
+        <v>FaxNew</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="2"/>
-        <v>EmailOld</v>
+        <v>FaxOld</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3267,19 +3321,19 @@
         <v>460</v>
       </c>
       <c r="B17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>IswwwChanged</v>
+        <v>IsEmailChanged</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
-        <v>wwwNew</v>
+        <v>EmailNew</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="2"/>
-        <v>wwwOld</v>
+        <v>EmailOld</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3287,19 +3341,19 @@
         <v>460</v>
       </c>
       <c r="B18" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrPositionChanged</v>
+        <v>IswwwChanged</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
-        <v>MgrPositionNew</v>
+        <v>wwwNew</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="2"/>
-        <v>MgrPositionOld</v>
+        <v>wwwOld</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3307,19 +3361,19 @@
         <v>460</v>
       </c>
       <c r="B19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrCountryISO3CodeChanged</v>
+        <v>IsMgrPositionChanged</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
-        <v>MgrCountryISO3CodeNew</v>
+        <v>MgrPositionNew</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="2"/>
-        <v>MgrCountryISO3CodeOld</v>
+        <v>MgrPositionOld</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3327,19 +3381,19 @@
         <v>460</v>
       </c>
       <c r="B20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrCountryNameUkrChanged</v>
+        <v>IsMgrCountryISO3CodeChanged</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
-        <v>MgrCountryNameUkrNew</v>
+        <v>MgrCountryISO3CodeNew</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="2"/>
-        <v>MgrCountryNameUkrOld</v>
+        <v>MgrCountryISO3CodeOld</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3347,19 +3401,19 @@
         <v>460</v>
       </c>
       <c r="B21" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrSurnameChanged</v>
+        <v>IsMgrCountryNameUkrChanged</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
-        <v>MgrSurnameNew</v>
+        <v>MgrCountryNameUkrNew</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="2"/>
-        <v>MgrSurnameOld</v>
+        <v>MgrCountryNameUkrOld</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3367,19 +3421,19 @@
         <v>460</v>
       </c>
       <c r="B22" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrNameChanged</v>
+        <v>IsMgrSurnameChanged</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
-        <v>MgrNameNew</v>
+        <v>MgrSurnameNew</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="2"/>
-        <v>MgrNameOld</v>
+        <v>MgrSurnameOld</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3387,19 +3441,19 @@
         <v>460</v>
       </c>
       <c r="B23" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrMiddleNameChanged</v>
+        <v>IsMgrNameChanged</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
-        <v>MgrMiddleNameNew</v>
+        <v>MgrNameNew</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="2"/>
-        <v>MgrMiddleNameOld</v>
+        <v>MgrNameOld</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3407,19 +3461,19 @@
         <v>460</v>
       </c>
       <c r="B24" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrSurnameAtBirthChanged</v>
+        <v>IsMgrMiddleNameChanged</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
-        <v>MgrSurnameAtBirthNew</v>
+        <v>MgrMiddleNameNew</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="2"/>
-        <v>MgrSurnameAtBirthOld</v>
+        <v>MgrMiddleNameOld</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3427,19 +3481,19 @@
         <v>460</v>
       </c>
       <c r="B25" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrTaxOrSocSecIDChanged</v>
+        <v>IsMgrSurnameAtBirthChanged</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
-        <v>MgrTaxOrSocSecIDNew</v>
+        <v>MgrSurnameAtBirthNew</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="2"/>
-        <v>MgrTaxOrSocSecIDOld</v>
+        <v>MgrSurnameAtBirthOld</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3447,59 +3501,59 @@
         <v>460</v>
       </c>
       <c r="B26" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrPassportIDChanged</v>
+        <v>IsMgrTaxOrSocSecIDChanged</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
-        <v>MgrPassportIDNew</v>
+        <v>MgrTaxOrSocSecIDNew</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="2"/>
-        <v>MgrPassportIDOld</v>
+        <v>MgrTaxOrSocSecIDOld</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="B27" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>IsMgrPassIssuedDateChanged</v>
+        <v>IsMgrPassportIDChanged</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
-        <v>MgrPassIssuedDateNew</v>
+        <v>MgrPassportIDNew</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="2"/>
-        <v>MgrPassIssuedDateOld</v>
+        <v>MgrPassportIDOld</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>460</v>
+        <v>486</v>
       </c>
       <c r="B28" t="s">
-        <v>568</v>
+        <v>487</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>IsRaionChanged</v>
+        <v>IsMgrPassIssuedDateChanged</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" ref="D28:D33" si="3">B28&amp;"New"</f>
-        <v>RaionNew</v>
+        <f t="shared" si="1"/>
+        <v>MgrPassIssuedDateNew</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" ref="E28:E33" si="4">B28&amp;"Old"</f>
-        <v>RaionOld</v>
+        <f t="shared" si="2"/>
+        <v>MgrPassIssuedDateOld</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3507,19 +3561,19 @@
         <v>460</v>
       </c>
       <c r="B29" t="s">
-        <v>569</v>
+        <v>592</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>IsZipCodeChanged</v>
+        <v>IsOblastChanged</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="3"/>
-        <v>ZipCodeNew</v>
+        <f t="shared" si="1"/>
+        <v>OblastNew</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="4"/>
-        <v>ZipCodeOld</v>
+        <f t="shared" si="2"/>
+        <v>OblastOld</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3527,19 +3581,19 @@
         <v>460</v>
       </c>
       <c r="B30" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>IsCityChanged</v>
+        <v>IsRaionChanged</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="3"/>
-        <v>CityNew</v>
+        <f t="shared" ref="D30:D35" si="3">B30&amp;"New"</f>
+        <v>RaionNew</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="4"/>
-        <v>CityOld</v>
+        <f t="shared" ref="E30:E35" si="4">B30&amp;"Old"</f>
+        <v>RaionOld</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3547,19 +3601,19 @@
         <v>460</v>
       </c>
       <c r="B31" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>IsStreetChanged</v>
+        <v>IsZipCodeChanged</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="3"/>
-        <v>StreetNew</v>
+        <v>ZipCodeNew</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="4"/>
-        <v>StreetOld</v>
+        <v>ZipCodeOld</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3567,19 +3621,19 @@
         <v>460</v>
       </c>
       <c r="B32" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>IsHouseNrChanged</v>
+        <v>IsCityChanged</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="3"/>
-        <v>HouseNrNew</v>
+        <v>CityNew</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="4"/>
-        <v>HouseNrOld</v>
+        <v>CityOld</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3587,19 +3641,99 @@
         <v>460</v>
       </c>
       <c r="B33" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>IsApptOfficeNrChanged</v>
+        <v>IsStreetChanged</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="3"/>
-        <v>ApptOfficeNrNew</v>
+        <v>StreetNew</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="4"/>
+        <v>StreetOld</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>460</v>
+      </c>
+      <c r="B34" t="s">
+        <v>572</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>IsHouseNrChanged</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="3"/>
+        <v>HouseNrNew</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="4"/>
+        <v>HouseNrOld</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>460</v>
+      </c>
+      <c r="B35" t="s">
+        <v>573</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>IsApptOfficeNrChanged</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="3"/>
+        <v>ApptOfficeNrNew</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="4"/>
         <v>ApptOfficeNrOld</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>460</v>
+      </c>
+      <c r="B36" t="s">
+        <v>602</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" ref="C36" si="5">"Is" &amp; B36 &amp;"Changed"</f>
+        <v>IsOperationsListingChanged</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" ref="D36" si="6">B36&amp;"New"</f>
+        <v>OperationsListingNew</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" ref="E36" si="7">B36&amp;"Old"</f>
+        <v>OperationsListingOld</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>313</v>
+      </c>
+      <c r="B37" t="s">
+        <v>606</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" ref="C37" si="8">"Is" &amp; B37 &amp;"Changed"</f>
+        <v>IsStatusChanged</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" ref="D37" si="9">B37&amp;"New"</f>
+        <v>StatusNew</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" ref="E37" si="10">B37&amp;"Old"</f>
+        <v>StatusOld</v>
       </c>
     </row>
   </sheetData>
@@ -10170,10 +10304,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:E37"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10937,17 +11071,105 @@
       <c r="A37" t="s">
         <v>401</v>
       </c>
+      <c r="B37" t="str">
+        <f t="shared" ref="B37:B41" si="13">"List"&amp;TRIM(A37)</f>
+        <v>ListBankAssociatedPersonsCode315p</v>
+      </c>
       <c r="C37" t="str">
-        <f t="shared" ref="C37" si="13">"public List&lt;EnumType&gt; "&amp;B37 &amp;"() { return EnumType.GetEnumList(typeof("&amp;A37&amp;")); }"</f>
-        <v>public List&lt;EnumType&gt; () { return EnumType.GetEnumList(typeof(BankAssociatedPersonsCode315p)); }</v>
+        <f t="shared" ref="C37:C41" si="14">"public List&lt;EnumType&gt; "&amp;B37 &amp;"() { return EnumType.GetEnumList(typeof("&amp;A37&amp;")); }"</f>
+        <v>public List&lt;EnumType&gt; ListBankAssociatedPersonsCode315p() { return EnumType.GetEnumList(typeof(BankAssociatedPersonsCode315p)); }</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" ref="D37" si="14">A37&amp;"List"</f>
+        <f t="shared" ref="D37:D41" si="15">A37&amp;"List"</f>
         <v>BankAssociatedPersonsCode315pList</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" ref="E37" si="15">"public static List&lt;EnumType&gt; "&amp;D37 &amp;" { get { return EnumType.GetEnumList(typeof("&amp;A37&amp;")); }}"</f>
+        <f t="shared" ref="E37:E41" si="16">"public static List&lt;EnumType&gt; "&amp;D37 &amp;" { get { return EnumType.GetEnumList(typeof("&amp;A37&amp;")); }}"</f>
         <v>public static List&lt;EnumType&gt; BankAssociatedPersonsCode315pList { get { return EnumType.GetEnumList(typeof(BankAssociatedPersonsCode315p)); }}</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>420</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="13"/>
+        <v>ListGeneralFXLicenseActivityType</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="14"/>
+        <v>public List&lt;EnumType&gt; ListGeneralFXLicenseActivityType() { return EnumType.GetEnumList(typeof(GeneralFXLicenseActivityType)); }</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="15"/>
+        <v>GeneralFXLicenseActivityTypeList</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="16"/>
+        <v>public static List&lt;EnumType&gt; GeneralFXLicenseActivityTypeList { get { return EnumType.GetEnumList(typeof(GeneralFXLicenseActivityType)); }}</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>439</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="13"/>
+        <v>ListProfessionalStockMarketActivityType</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="14"/>
+        <v>public List&lt;EnumType&gt; ListProfessionalStockMarketActivityType() { return EnumType.GetEnumList(typeof(ProfessionalStockMarketActivityType)); }</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="15"/>
+        <v>ProfessionalStockMarketActivityTypeList</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="16"/>
+        <v>public static List&lt;EnumType&gt; ProfessionalStockMarketActivityTypeList { get { return EnumType.GetEnumList(typeof(ProfessionalStockMarketActivityType)); }}</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>600</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="13"/>
+        <v>ListFinActivitySvcInstrumentActionType</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="14"/>
+        <v>public List&lt;EnumType&gt; ListFinActivitySvcInstrumentActionType() { return EnumType.GetEnumList(typeof(FinActivitySvcInstrumentActionType)); }</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="15"/>
+        <v>FinActivitySvcInstrumentActionTypeList</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="16"/>
+        <v>public static List&lt;EnumType&gt; FinActivitySvcInstrumentActionTypeList { get { return EnumType.GetEnumList(typeof(FinActivitySvcInstrumentActionType)); }}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>601</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="13"/>
+        <v>ListFinActivitySvcInstrumentType</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="14"/>
+        <v>public List&lt;EnumType&gt; ListFinActivitySvcInstrumentType() { return EnumType.GetEnumList(typeof(FinActivitySvcInstrumentType)); }</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="15"/>
+        <v>FinActivitySvcInstrumentTypeList</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="16"/>
+        <v>public static List&lt;EnumType&gt; FinActivitySvcInstrumentTypeList { get { return EnumType.GetEnumList(typeof(FinActivitySvcInstrumentType)); }}</v>
       </c>
     </row>
   </sheetData>
@@ -10963,8 +11185,8 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B44"/>
+    <sheetView topLeftCell="XEB2" workbookViewId="0">
+      <selection activeCell="XFD2" sqref="XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11374,10 +11596,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M114"/>
+  <dimension ref="A1:M126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55:L114"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="K124" sqref="K124:L126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12186,15 +12408,15 @@
         <v>488</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" ref="J19:J100" si="24">"_"&amp;I19</f>
+        <f t="shared" ref="J19:J106" si="24">"_"&amp;I19</f>
         <v>_IsParentIDChanged</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" ref="K19:K100" si="25">"private " &amp; H19 &amp; " " &amp; J19 &amp; ";"</f>
+        <f t="shared" ref="K19:K106" si="25">"private " &amp; H19 &amp; " " &amp; J19 &amp; ";"</f>
         <v>private bool _IsParentIDChanged;</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" ref="L19:L100" si="26">G19&amp; " " &amp;H19&amp; " " &amp;I19 &amp; " { get { return " &amp; J19 &amp; "; } set { " &amp;J19 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I19 &amp; CHAR(34) &amp; "); } }"</f>
+        <f t="shared" ref="L19:L106" si="26">G19&amp; " " &amp;H19&amp; " " &amp;I19 &amp; " { get { return " &amp; J19 &amp; "; } set { " &amp;J19 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I19 &amp; CHAR(34) &amp; "); } }"</f>
         <v>public bool IsParentIDChanged { get { return _IsParentIDChanged; } set { _IsParentIDChanged = value; OnPropertyChanged("IsParentIDChanged"); } }</v>
       </c>
     </row>
@@ -13008,22 +13230,22 @@
         <v>567</v>
       </c>
       <c r="H55" t="s">
-        <v>566</v>
+        <v>460</v>
       </c>
       <c r="I55" t="s">
-        <v>574</v>
+        <v>593</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" ref="J55:J72" si="27">"_"&amp;I55</f>
-        <v>_IsRaionChanged</v>
+        <f t="shared" ref="J55:J57" si="27">"_"&amp;I55</f>
+        <v>_IsOblastChanged</v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" ref="K55:K72" si="28">"private " &amp; H55 &amp; " " &amp; J55 &amp; ";"</f>
-        <v>private bool _IsRaionChanged;</v>
+        <f t="shared" ref="K55:K57" si="28">"private " &amp; H55 &amp; " " &amp; J55 &amp; ";"</f>
+        <v>private string _IsOblastChanged;</v>
       </c>
       <c r="L55" t="str">
-        <f t="shared" ref="L55:L72" si="29">G55&amp; " " &amp;H55&amp; " " &amp;I55 &amp; " { get { return " &amp; J55 &amp; "; } set { " &amp;J55 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I55 &amp; CHAR(34) &amp; "); } }"</f>
-        <v>public bool IsRaionChanged { get { return _IsRaionChanged; } set { _IsRaionChanged = value; OnPropertyChanged("IsRaionChanged"); } }</v>
+        <f t="shared" ref="L55:L57" si="29">G55&amp; " " &amp;H55&amp; " " &amp;I55 &amp; " { get { return " &amp; J55 &amp; "; } set { " &amp;J55 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I55 &amp; CHAR(34) &amp; "); } }"</f>
+        <v>public string IsOblastChanged { get { return _IsOblastChanged; } set { _IsOblastChanged = value; OnPropertyChanged("IsOblastChanged"); } }</v>
       </c>
     </row>
     <row r="56" spans="7:12" x14ac:dyDescent="0.25">
@@ -13034,19 +13256,19 @@
         <v>460</v>
       </c>
       <c r="I56" t="s">
-        <v>575</v>
+        <v>594</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="27"/>
-        <v>_RaionNew</v>
+        <v>_OblastNew</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="28"/>
-        <v>private string _RaionNew;</v>
+        <v>private string _OblastNew;</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" si="29"/>
-        <v>public string RaionNew { get { return _RaionNew; } set { _RaionNew = value; OnPropertyChanged("RaionNew"); } }</v>
+        <v>public string OblastNew { get { return _OblastNew; } set { _OblastNew = value; OnPropertyChanged("OblastNew"); } }</v>
       </c>
     </row>
     <row r="57" spans="7:12" x14ac:dyDescent="0.25">
@@ -13057,19 +13279,19 @@
         <v>460</v>
       </c>
       <c r="I57" t="s">
-        <v>576</v>
+        <v>595</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="27"/>
-        <v>_RaionOld</v>
+        <v>_OblastOld</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="28"/>
-        <v>private string _RaionOld;</v>
+        <v>private string _OblastOld;</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" si="29"/>
-        <v>public string RaionOld { get { return _RaionOld; } set { _RaionOld = value; OnPropertyChanged("RaionOld"); } }</v>
+        <v>public string OblastOld { get { return _OblastOld; } set { _OblastOld = value; OnPropertyChanged("OblastOld"); } }</v>
       </c>
     </row>
     <row r="58" spans="7:12" x14ac:dyDescent="0.25">
@@ -13080,19 +13302,19 @@
         <v>566</v>
       </c>
       <c r="I58" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="27"/>
-        <v>_IsZipCodeChanged</v>
+        <f t="shared" ref="J58:J75" si="30">"_"&amp;I58</f>
+        <v>_IsRaionChanged</v>
       </c>
       <c r="K58" t="str">
-        <f t="shared" si="28"/>
-        <v>private bool _IsZipCodeChanged;</v>
+        <f t="shared" ref="K58:K75" si="31">"private " &amp; H58 &amp; " " &amp; J58 &amp; ";"</f>
+        <v>private bool _IsRaionChanged;</v>
       </c>
       <c r="L58" t="str">
-        <f t="shared" si="29"/>
-        <v>public bool IsZipCodeChanged { get { return _IsZipCodeChanged; } set { _IsZipCodeChanged = value; OnPropertyChanged("IsZipCodeChanged"); } }</v>
+        <f t="shared" ref="L58:L75" si="32">G58&amp; " " &amp;H58&amp; " " &amp;I58 &amp; " { get { return " &amp; J58 &amp; "; } set { " &amp;J58 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I58 &amp; CHAR(34) &amp; "); } }"</f>
+        <v>public bool IsRaionChanged { get { return _IsRaionChanged; } set { _IsRaionChanged = value; OnPropertyChanged("IsRaionChanged"); } }</v>
       </c>
     </row>
     <row r="59" spans="7:12" x14ac:dyDescent="0.25">
@@ -13103,19 +13325,19 @@
         <v>460</v>
       </c>
       <c r="I59" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="27"/>
-        <v>_ZipCodeNew</v>
+        <f t="shared" si="30"/>
+        <v>_RaionNew</v>
       </c>
       <c r="K59" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _ZipCodeNew;</v>
+        <f t="shared" si="31"/>
+        <v>private string _RaionNew;</v>
       </c>
       <c r="L59" t="str">
-        <f t="shared" si="29"/>
-        <v>public string ZipCodeNew { get { return _ZipCodeNew; } set { _ZipCodeNew = value; OnPropertyChanged("ZipCodeNew"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string RaionNew { get { return _RaionNew; } set { _RaionNew = value; OnPropertyChanged("RaionNew"); } }</v>
       </c>
     </row>
     <row r="60" spans="7:12" x14ac:dyDescent="0.25">
@@ -13126,19 +13348,19 @@
         <v>460</v>
       </c>
       <c r="I60" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="27"/>
-        <v>_ZipCodeOld</v>
+        <f t="shared" si="30"/>
+        <v>_RaionOld</v>
       </c>
       <c r="K60" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _ZipCodeOld;</v>
+        <f t="shared" si="31"/>
+        <v>private string _RaionOld;</v>
       </c>
       <c r="L60" t="str">
-        <f t="shared" si="29"/>
-        <v>public string ZipCodeOld { get { return _ZipCodeOld; } set { _ZipCodeOld = value; OnPropertyChanged("ZipCodeOld"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string RaionOld { get { return _RaionOld; } set { _RaionOld = value; OnPropertyChanged("RaionOld"); } }</v>
       </c>
     </row>
     <row r="61" spans="7:12" x14ac:dyDescent="0.25">
@@ -13149,19 +13371,19 @@
         <v>566</v>
       </c>
       <c r="I61" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" si="27"/>
-        <v>_IsCityChanged</v>
+        <f t="shared" si="30"/>
+        <v>_IsZipCodeChanged</v>
       </c>
       <c r="K61" t="str">
-        <f t="shared" si="28"/>
-        <v>private bool _IsCityChanged;</v>
+        <f t="shared" si="31"/>
+        <v>private bool _IsZipCodeChanged;</v>
       </c>
       <c r="L61" t="str">
-        <f t="shared" si="29"/>
-        <v>public bool IsCityChanged { get { return _IsCityChanged; } set { _IsCityChanged = value; OnPropertyChanged("IsCityChanged"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public bool IsZipCodeChanged { get { return _IsZipCodeChanged; } set { _IsZipCodeChanged = value; OnPropertyChanged("IsZipCodeChanged"); } }</v>
       </c>
     </row>
     <row r="62" spans="7:12" x14ac:dyDescent="0.25">
@@ -13172,19 +13394,19 @@
         <v>460</v>
       </c>
       <c r="I62" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" si="27"/>
-        <v>_CityNew</v>
+        <f t="shared" si="30"/>
+        <v>_ZipCodeNew</v>
       </c>
       <c r="K62" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _CityNew;</v>
+        <f t="shared" si="31"/>
+        <v>private string _ZipCodeNew;</v>
       </c>
       <c r="L62" t="str">
-        <f t="shared" si="29"/>
-        <v>public string CityNew { get { return _CityNew; } set { _CityNew = value; OnPropertyChanged("CityNew"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string ZipCodeNew { get { return _ZipCodeNew; } set { _ZipCodeNew = value; OnPropertyChanged("ZipCodeNew"); } }</v>
       </c>
     </row>
     <row r="63" spans="7:12" x14ac:dyDescent="0.25">
@@ -13195,19 +13417,19 @@
         <v>460</v>
       </c>
       <c r="I63" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" si="27"/>
-        <v>_CityOld</v>
+        <f t="shared" si="30"/>
+        <v>_ZipCodeOld</v>
       </c>
       <c r="K63" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _CityOld;</v>
+        <f t="shared" si="31"/>
+        <v>private string _ZipCodeOld;</v>
       </c>
       <c r="L63" t="str">
-        <f t="shared" si="29"/>
-        <v>public string CityOld { get { return _CityOld; } set { _CityOld = value; OnPropertyChanged("CityOld"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string ZipCodeOld { get { return _ZipCodeOld; } set { _ZipCodeOld = value; OnPropertyChanged("ZipCodeOld"); } }</v>
       </c>
     </row>
     <row r="64" spans="7:12" x14ac:dyDescent="0.25">
@@ -13218,19 +13440,19 @@
         <v>566</v>
       </c>
       <c r="I64" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" si="27"/>
-        <v>_IsStreetChanged</v>
+        <f t="shared" si="30"/>
+        <v>_IsCityChanged</v>
       </c>
       <c r="K64" t="str">
-        <f t="shared" si="28"/>
-        <v>private bool _IsStreetChanged;</v>
+        <f t="shared" si="31"/>
+        <v>private bool _IsCityChanged;</v>
       </c>
       <c r="L64" t="str">
-        <f t="shared" si="29"/>
-        <v>public bool IsStreetChanged { get { return _IsStreetChanged; } set { _IsStreetChanged = value; OnPropertyChanged("IsStreetChanged"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public bool IsCityChanged { get { return _IsCityChanged; } set { _IsCityChanged = value; OnPropertyChanged("IsCityChanged"); } }</v>
       </c>
     </row>
     <row r="65" spans="7:12" x14ac:dyDescent="0.25">
@@ -13241,19 +13463,19 @@
         <v>460</v>
       </c>
       <c r="I65" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" si="27"/>
-        <v>_StreetNew</v>
+        <f t="shared" si="30"/>
+        <v>_CityNew</v>
       </c>
       <c r="K65" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _StreetNew;</v>
+        <f t="shared" si="31"/>
+        <v>private string _CityNew;</v>
       </c>
       <c r="L65" t="str">
-        <f t="shared" si="29"/>
-        <v>public string StreetNew { get { return _StreetNew; } set { _StreetNew = value; OnPropertyChanged("StreetNew"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string CityNew { get { return _CityNew; } set { _CityNew = value; OnPropertyChanged("CityNew"); } }</v>
       </c>
     </row>
     <row r="66" spans="7:12" x14ac:dyDescent="0.25">
@@ -13264,19 +13486,19 @@
         <v>460</v>
       </c>
       <c r="I66" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" si="27"/>
-        <v>_StreetOld</v>
+        <f t="shared" si="30"/>
+        <v>_CityOld</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _StreetOld;</v>
+        <f t="shared" si="31"/>
+        <v>private string _CityOld;</v>
       </c>
       <c r="L66" t="str">
-        <f t="shared" si="29"/>
-        <v>public string StreetOld { get { return _StreetOld; } set { _StreetOld = value; OnPropertyChanged("StreetOld"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string CityOld { get { return _CityOld; } set { _CityOld = value; OnPropertyChanged("CityOld"); } }</v>
       </c>
     </row>
     <row r="67" spans="7:12" x14ac:dyDescent="0.25">
@@ -13287,19 +13509,19 @@
         <v>566</v>
       </c>
       <c r="I67" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" si="27"/>
-        <v>_IsHouseNrChanged</v>
+        <f t="shared" si="30"/>
+        <v>_IsStreetChanged</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" si="28"/>
-        <v>private bool _IsHouseNrChanged;</v>
+        <f t="shared" si="31"/>
+        <v>private bool _IsStreetChanged;</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" si="29"/>
-        <v>public bool IsHouseNrChanged { get { return _IsHouseNrChanged; } set { _IsHouseNrChanged = value; OnPropertyChanged("IsHouseNrChanged"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public bool IsStreetChanged { get { return _IsStreetChanged; } set { _IsStreetChanged = value; OnPropertyChanged("IsStreetChanged"); } }</v>
       </c>
     </row>
     <row r="68" spans="7:12" x14ac:dyDescent="0.25">
@@ -13310,19 +13532,19 @@
         <v>460</v>
       </c>
       <c r="I68" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" si="27"/>
-        <v>_HouseNrNew</v>
+        <f t="shared" si="30"/>
+        <v>_StreetNew</v>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _HouseNrNew;</v>
+        <f t="shared" si="31"/>
+        <v>private string _StreetNew;</v>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="29"/>
-        <v>public string HouseNrNew { get { return _HouseNrNew; } set { _HouseNrNew = value; OnPropertyChanged("HouseNrNew"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string StreetNew { get { return _StreetNew; } set { _StreetNew = value; OnPropertyChanged("StreetNew"); } }</v>
       </c>
     </row>
     <row r="69" spans="7:12" x14ac:dyDescent="0.25">
@@ -13333,19 +13555,19 @@
         <v>460</v>
       </c>
       <c r="I69" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" si="27"/>
-        <v>_HouseNrOld</v>
+        <f t="shared" si="30"/>
+        <v>_StreetOld</v>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _HouseNrOld;</v>
+        <f t="shared" si="31"/>
+        <v>private string _StreetOld;</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="29"/>
-        <v>public string HouseNrOld { get { return _HouseNrOld; } set { _HouseNrOld = value; OnPropertyChanged("HouseNrOld"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string StreetOld { get { return _StreetOld; } set { _StreetOld = value; OnPropertyChanged("StreetOld"); } }</v>
       </c>
     </row>
     <row r="70" spans="7:12" x14ac:dyDescent="0.25">
@@ -13356,19 +13578,19 @@
         <v>566</v>
       </c>
       <c r="I70" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" si="27"/>
-        <v>_IsApptOfficeNrChanged</v>
+        <f t="shared" si="30"/>
+        <v>_IsHouseNrChanged</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="28"/>
-        <v>private bool _IsApptOfficeNrChanged;</v>
+        <f t="shared" si="31"/>
+        <v>private bool _IsHouseNrChanged;</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" si="29"/>
-        <v>public bool IsApptOfficeNrChanged { get { return _IsApptOfficeNrChanged; } set { _IsApptOfficeNrChanged = value; OnPropertyChanged("IsApptOfficeNrChanged"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public bool IsHouseNrChanged { get { return _IsHouseNrChanged; } set { _IsHouseNrChanged = value; OnPropertyChanged("IsHouseNrChanged"); } }</v>
       </c>
     </row>
     <row r="71" spans="7:12" x14ac:dyDescent="0.25">
@@ -13379,19 +13601,19 @@
         <v>460</v>
       </c>
       <c r="I71" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" si="27"/>
-        <v>_ApptOfficeNrNew</v>
+        <f t="shared" si="30"/>
+        <v>_HouseNrNew</v>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _ApptOfficeNrNew;</v>
+        <f t="shared" si="31"/>
+        <v>private string _HouseNrNew;</v>
       </c>
       <c r="L71" t="str">
-        <f t="shared" si="29"/>
-        <v>public string ApptOfficeNrNew { get { return _ApptOfficeNrNew; } set { _ApptOfficeNrNew = value; OnPropertyChanged("ApptOfficeNrNew"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string HouseNrNew { get { return _HouseNrNew; } set { _HouseNrNew = value; OnPropertyChanged("HouseNrNew"); } }</v>
       </c>
     </row>
     <row r="72" spans="7:12" x14ac:dyDescent="0.25">
@@ -13402,19 +13624,19 @@
         <v>460</v>
       </c>
       <c r="I72" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" si="27"/>
-        <v>_ApptOfficeNrOld</v>
+        <f t="shared" si="30"/>
+        <v>_HouseNrOld</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="28"/>
-        <v>private string _ApptOfficeNrOld;</v>
+        <f t="shared" si="31"/>
+        <v>private string _HouseNrOld;</v>
       </c>
       <c r="L72" t="str">
-        <f t="shared" si="29"/>
-        <v>public string ApptOfficeNrOld { get { return _ApptOfficeNrOld; } set { _ApptOfficeNrOld = value; OnPropertyChanged("ApptOfficeNrOld"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string HouseNrOld { get { return _HouseNrOld; } set { _HouseNrOld = value; OnPropertyChanged("HouseNrOld"); } }</v>
       </c>
     </row>
     <row r="73" spans="7:12" x14ac:dyDescent="0.25">
@@ -13425,19 +13647,19 @@
         <v>566</v>
       </c>
       <c r="I73" t="s">
-        <v>512</v>
+        <v>589</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" si="24"/>
-        <v>_IsDialCodeChanged</v>
+        <f t="shared" si="30"/>
+        <v>_IsApptOfficeNrChanged</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="25"/>
-        <v>private bool _IsDialCodeChanged;</v>
+        <f t="shared" si="31"/>
+        <v>private bool _IsApptOfficeNrChanged;</v>
       </c>
       <c r="L73" t="str">
-        <f t="shared" si="26"/>
-        <v>public bool IsDialCodeChanged { get { return _IsDialCodeChanged; } set { _IsDialCodeChanged = value; OnPropertyChanged("IsDialCodeChanged"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public bool IsApptOfficeNrChanged { get { return _IsApptOfficeNrChanged; } set { _IsApptOfficeNrChanged = value; OnPropertyChanged("IsApptOfficeNrChanged"); } }</v>
       </c>
     </row>
     <row r="74" spans="7:12" x14ac:dyDescent="0.25">
@@ -13448,19 +13670,19 @@
         <v>460</v>
       </c>
       <c r="I74" t="s">
-        <v>552</v>
+        <v>590</v>
       </c>
       <c r="J74" t="str">
-        <f t="shared" si="24"/>
-        <v>_DialCodeNew</v>
+        <f t="shared" si="30"/>
+        <v>_ApptOfficeNrNew</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="25"/>
-        <v>private string _DialCodeNew;</v>
+        <f t="shared" si="31"/>
+        <v>private string _ApptOfficeNrNew;</v>
       </c>
       <c r="L74" t="str">
-        <f t="shared" si="26"/>
-        <v>public string DialCodeNew { get { return _DialCodeNew; } set { _DialCodeNew = value; OnPropertyChanged("DialCodeNew"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string ApptOfficeNrNew { get { return _ApptOfficeNrNew; } set { _ApptOfficeNrNew = value; OnPropertyChanged("ApptOfficeNrNew"); } }</v>
       </c>
     </row>
     <row r="75" spans="7:12" x14ac:dyDescent="0.25">
@@ -13471,19 +13693,19 @@
         <v>460</v>
       </c>
       <c r="I75" t="s">
-        <v>513</v>
+        <v>591</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" si="24"/>
-        <v>_DialCodeOld</v>
+        <f t="shared" si="30"/>
+        <v>_ApptOfficeNrOld</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="25"/>
-        <v>private string _DialCodeOld;</v>
+        <f t="shared" si="31"/>
+        <v>private string _ApptOfficeNrOld;</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="26"/>
-        <v>public string DialCodeOld { get { return _DialCodeOld; } set { _DialCodeOld = value; OnPropertyChanged("DialCodeOld"); } }</v>
+        <f t="shared" si="32"/>
+        <v>public string ApptOfficeNrOld { get { return _ApptOfficeNrOld; } set { _ApptOfficeNrOld = value; OnPropertyChanged("ApptOfficeNrOld"); } }</v>
       </c>
     </row>
     <row r="76" spans="7:12" x14ac:dyDescent="0.25">
@@ -13494,19 +13716,19 @@
         <v>566</v>
       </c>
       <c r="I76" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="J76" t="str">
         <f t="shared" si="24"/>
-        <v>_IsFaxChanged</v>
+        <v>_IsDialCodeChanged</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" si="25"/>
-        <v>private bool _IsFaxChanged;</v>
+        <v>private bool _IsDialCodeChanged;</v>
       </c>
       <c r="L76" t="str">
         <f t="shared" si="26"/>
-        <v>public bool IsFaxChanged { get { return _IsFaxChanged; } set { _IsFaxChanged = value; OnPropertyChanged("IsFaxChanged"); } }</v>
+        <v>public bool IsDialCodeChanged { get { return _IsDialCodeChanged; } set { _IsDialCodeChanged = value; OnPropertyChanged("IsDialCodeChanged"); } }</v>
       </c>
     </row>
     <row r="77" spans="7:12" x14ac:dyDescent="0.25">
@@ -13517,19 +13739,19 @@
         <v>460</v>
       </c>
       <c r="I77" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J77" t="str">
         <f t="shared" si="24"/>
-        <v>_FaxNew</v>
+        <v>_DialCodeNew</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="25"/>
-        <v>private string _FaxNew;</v>
+        <v>private string _DialCodeNew;</v>
       </c>
       <c r="L77" t="str">
         <f t="shared" si="26"/>
-        <v>public string FaxNew { get { return _FaxNew; } set { _FaxNew = value; OnPropertyChanged("FaxNew"); } }</v>
+        <v>public string DialCodeNew { get { return _DialCodeNew; } set { _DialCodeNew = value; OnPropertyChanged("DialCodeNew"); } }</v>
       </c>
     </row>
     <row r="78" spans="7:12" x14ac:dyDescent="0.25">
@@ -13540,19 +13762,19 @@
         <v>460</v>
       </c>
       <c r="I78" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J78" t="str">
         <f t="shared" si="24"/>
-        <v>_FaxOld</v>
+        <v>_DialCodeOld</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="25"/>
-        <v>private string _FaxOld;</v>
+        <v>private string _DialCodeOld;</v>
       </c>
       <c r="L78" t="str">
         <f t="shared" si="26"/>
-        <v>public string FaxOld { get { return _FaxOld; } set { _FaxOld = value; OnPropertyChanged("FaxOld"); } }</v>
+        <v>public string DialCodeOld { get { return _DialCodeOld; } set { _DialCodeOld = value; OnPropertyChanged("DialCodeOld"); } }</v>
       </c>
     </row>
     <row r="79" spans="7:12" x14ac:dyDescent="0.25">
@@ -13563,19 +13785,19 @@
         <v>566</v>
       </c>
       <c r="I79" t="s">
-        <v>516</v>
+        <v>597</v>
       </c>
       <c r="J79" t="str">
-        <f t="shared" si="24"/>
-        <v>_IsEmailChanged</v>
+        <f t="shared" ref="J79:J81" si="33">"_"&amp;I79</f>
+        <v>_IsPhoneChanged</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="25"/>
-        <v>private bool _IsEmailChanged;</v>
+        <f t="shared" ref="K79:K81" si="34">"private " &amp; H79 &amp; " " &amp; J79 &amp; ";"</f>
+        <v>private bool _IsPhoneChanged;</v>
       </c>
       <c r="L79" t="str">
-        <f t="shared" si="26"/>
-        <v>public bool IsEmailChanged { get { return _IsEmailChanged; } set { _IsEmailChanged = value; OnPropertyChanged("IsEmailChanged"); } }</v>
+        <f t="shared" ref="L79:L81" si="35">G79&amp; " " &amp;H79&amp; " " &amp;I79 &amp; " { get { return " &amp; J79 &amp; "; } set { " &amp;J79 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I79 &amp; CHAR(34) &amp; "); } }"</f>
+        <v>public bool IsPhoneChanged { get { return _IsPhoneChanged; } set { _IsPhoneChanged = value; OnPropertyChanged("IsPhoneChanged"); } }</v>
       </c>
     </row>
     <row r="80" spans="7:12" x14ac:dyDescent="0.25">
@@ -13586,19 +13808,19 @@
         <v>460</v>
       </c>
       <c r="I80" t="s">
-        <v>554</v>
+        <v>598</v>
       </c>
       <c r="J80" t="str">
-        <f t="shared" si="24"/>
-        <v>_EmailNew</v>
+        <f t="shared" si="33"/>
+        <v>_PhoneNew</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="25"/>
-        <v>private string _EmailNew;</v>
+        <f t="shared" si="34"/>
+        <v>private string _PhoneNew;</v>
       </c>
       <c r="L80" t="str">
-        <f t="shared" si="26"/>
-        <v>public string EmailNew { get { return _EmailNew; } set { _EmailNew = value; OnPropertyChanged("EmailNew"); } }</v>
+        <f t="shared" si="35"/>
+        <v>public string PhoneNew { get { return _PhoneNew; } set { _PhoneNew = value; OnPropertyChanged("PhoneNew"); } }</v>
       </c>
     </row>
     <row r="81" spans="7:12" x14ac:dyDescent="0.25">
@@ -13609,19 +13831,19 @@
         <v>460</v>
       </c>
       <c r="I81" t="s">
-        <v>517</v>
+        <v>599</v>
       </c>
       <c r="J81" t="str">
-        <f t="shared" si="24"/>
-        <v>_EmailOld</v>
+        <f t="shared" si="33"/>
+        <v>_PhoneOld</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="25"/>
-        <v>private string _EmailOld;</v>
+        <f t="shared" si="34"/>
+        <v>private string _PhoneOld;</v>
       </c>
       <c r="L81" t="str">
-        <f t="shared" si="26"/>
-        <v>public string EmailOld { get { return _EmailOld; } set { _EmailOld = value; OnPropertyChanged("EmailOld"); } }</v>
+        <f t="shared" si="35"/>
+        <v>public string PhoneOld { get { return _PhoneOld; } set { _PhoneOld = value; OnPropertyChanged("PhoneOld"); } }</v>
       </c>
     </row>
     <row r="82" spans="7:12" x14ac:dyDescent="0.25">
@@ -13632,19 +13854,19 @@
         <v>566</v>
       </c>
       <c r="I82" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="J82" t="str">
         <f t="shared" si="24"/>
-        <v>_IswwwChanged</v>
+        <v>_IsFaxChanged</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="25"/>
-        <v>private bool _IswwwChanged;</v>
+        <v>private bool _IsFaxChanged;</v>
       </c>
       <c r="L82" t="str">
         <f t="shared" si="26"/>
-        <v>public bool IswwwChanged { get { return _IswwwChanged; } set { _IswwwChanged = value; OnPropertyChanged("IswwwChanged"); } }</v>
+        <v>public bool IsFaxChanged { get { return _IsFaxChanged; } set { _IsFaxChanged = value; OnPropertyChanged("IsFaxChanged"); } }</v>
       </c>
     </row>
     <row r="83" spans="7:12" x14ac:dyDescent="0.25">
@@ -13655,19 +13877,19 @@
         <v>460</v>
       </c>
       <c r="I83" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J83" t="str">
         <f t="shared" si="24"/>
-        <v>_wwwNew</v>
+        <v>_FaxNew</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="25"/>
-        <v>private string _wwwNew;</v>
+        <v>private string _FaxNew;</v>
       </c>
       <c r="L83" t="str">
         <f t="shared" si="26"/>
-        <v>public string wwwNew { get { return _wwwNew; } set { _wwwNew = value; OnPropertyChanged("wwwNew"); } }</v>
+        <v>public string FaxNew { get { return _FaxNew; } set { _FaxNew = value; OnPropertyChanged("FaxNew"); } }</v>
       </c>
     </row>
     <row r="84" spans="7:12" x14ac:dyDescent="0.25">
@@ -13678,19 +13900,19 @@
         <v>460</v>
       </c>
       <c r="I84" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="J84" t="str">
         <f t="shared" si="24"/>
-        <v>_wwwOld</v>
+        <v>_FaxOld</v>
       </c>
       <c r="K84" t="str">
         <f t="shared" si="25"/>
-        <v>private string _wwwOld;</v>
+        <v>private string _FaxOld;</v>
       </c>
       <c r="L84" t="str">
         <f t="shared" si="26"/>
-        <v>public string wwwOld { get { return _wwwOld; } set { _wwwOld = value; OnPropertyChanged("wwwOld"); } }</v>
+        <v>public string FaxOld { get { return _FaxOld; } set { _FaxOld = value; OnPropertyChanged("FaxOld"); } }</v>
       </c>
     </row>
     <row r="85" spans="7:12" x14ac:dyDescent="0.25">
@@ -13701,19 +13923,19 @@
         <v>566</v>
       </c>
       <c r="I85" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="J85" t="str">
         <f t="shared" si="24"/>
-        <v>_IsMgrPositionChanged</v>
+        <v>_IsEmailChanged</v>
       </c>
       <c r="K85" t="str">
         <f t="shared" si="25"/>
-        <v>private bool _IsMgrPositionChanged;</v>
+        <v>private bool _IsEmailChanged;</v>
       </c>
       <c r="L85" t="str">
         <f t="shared" si="26"/>
-        <v>public bool IsMgrPositionChanged { get { return _IsMgrPositionChanged; } set { _IsMgrPositionChanged = value; OnPropertyChanged("IsMgrPositionChanged"); } }</v>
+        <v>public bool IsEmailChanged { get { return _IsEmailChanged; } set { _IsEmailChanged = value; OnPropertyChanged("IsEmailChanged"); } }</v>
       </c>
     </row>
     <row r="86" spans="7:12" x14ac:dyDescent="0.25">
@@ -13724,19 +13946,19 @@
         <v>460</v>
       </c>
       <c r="I86" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="J86" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrPositionNew</v>
+        <v>_EmailNew</v>
       </c>
       <c r="K86" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrPositionNew;</v>
+        <v>private string _EmailNew;</v>
       </c>
       <c r="L86" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrPositionNew { get { return _MgrPositionNew; } set { _MgrPositionNew = value; OnPropertyChanged("MgrPositionNew"); } }</v>
+        <v>public string EmailNew { get { return _EmailNew; } set { _EmailNew = value; OnPropertyChanged("EmailNew"); } }</v>
       </c>
     </row>
     <row r="87" spans="7:12" x14ac:dyDescent="0.25">
@@ -13747,19 +13969,19 @@
         <v>460</v>
       </c>
       <c r="I87" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="J87" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrPositionOld</v>
+        <v>_EmailOld</v>
       </c>
       <c r="K87" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrPositionOld;</v>
+        <v>private string _EmailOld;</v>
       </c>
       <c r="L87" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrPositionOld { get { return _MgrPositionOld; } set { _MgrPositionOld = value; OnPropertyChanged("MgrPositionOld"); } }</v>
+        <v>public string EmailOld { get { return _EmailOld; } set { _EmailOld = value; OnPropertyChanged("EmailOld"); } }</v>
       </c>
     </row>
     <row r="88" spans="7:12" x14ac:dyDescent="0.25">
@@ -13770,19 +13992,19 @@
         <v>566</v>
       </c>
       <c r="I88" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="J88" t="str">
         <f t="shared" si="24"/>
-        <v>_IsMgrCountryISO3CodeChanged</v>
+        <v>_IswwwChanged</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="25"/>
-        <v>private bool _IsMgrCountryISO3CodeChanged;</v>
+        <v>private bool _IswwwChanged;</v>
       </c>
       <c r="L88" t="str">
         <f t="shared" si="26"/>
-        <v>public bool IsMgrCountryISO3CodeChanged { get { return _IsMgrCountryISO3CodeChanged; } set { _IsMgrCountryISO3CodeChanged = value; OnPropertyChanged("IsMgrCountryISO3CodeChanged"); } }</v>
+        <v>public bool IswwwChanged { get { return _IswwwChanged; } set { _IswwwChanged = value; OnPropertyChanged("IswwwChanged"); } }</v>
       </c>
     </row>
     <row r="89" spans="7:12" x14ac:dyDescent="0.25">
@@ -13793,19 +14015,19 @@
         <v>460</v>
       </c>
       <c r="I89" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="J89" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrCountryISO3CodeNew</v>
+        <v>_wwwNew</v>
       </c>
       <c r="K89" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrCountryISO3CodeNew;</v>
+        <v>private string _wwwNew;</v>
       </c>
       <c r="L89" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrCountryISO3CodeNew { get { return _MgrCountryISO3CodeNew; } set { _MgrCountryISO3CodeNew = value; OnPropertyChanged("MgrCountryISO3CodeNew"); } }</v>
+        <v>public string wwwNew { get { return _wwwNew; } set { _wwwNew = value; OnPropertyChanged("wwwNew"); } }</v>
       </c>
     </row>
     <row r="90" spans="7:12" x14ac:dyDescent="0.25">
@@ -13816,19 +14038,19 @@
         <v>460</v>
       </c>
       <c r="I90" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="J90" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrCountryISO3CodeOld</v>
+        <v>_wwwOld</v>
       </c>
       <c r="K90" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrCountryISO3CodeOld;</v>
+        <v>private string _wwwOld;</v>
       </c>
       <c r="L90" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrCountryISO3CodeOld { get { return _MgrCountryISO3CodeOld; } set { _MgrCountryISO3CodeOld = value; OnPropertyChanged("MgrCountryISO3CodeOld"); } }</v>
+        <v>public string wwwOld { get { return _wwwOld; } set { _wwwOld = value; OnPropertyChanged("wwwOld"); } }</v>
       </c>
     </row>
     <row r="91" spans="7:12" x14ac:dyDescent="0.25">
@@ -13839,19 +14061,19 @@
         <v>566</v>
       </c>
       <c r="I91" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="J91" t="str">
         <f t="shared" si="24"/>
-        <v>_IsMgrCountryNameUkrChanged</v>
+        <v>_IsMgrPositionChanged</v>
       </c>
       <c r="K91" t="str">
         <f t="shared" si="25"/>
-        <v>private bool _IsMgrCountryNameUkrChanged;</v>
+        <v>private bool _IsMgrPositionChanged;</v>
       </c>
       <c r="L91" t="str">
         <f t="shared" si="26"/>
-        <v>public bool IsMgrCountryNameUkrChanged { get { return _IsMgrCountryNameUkrChanged; } set { _IsMgrCountryNameUkrChanged = value; OnPropertyChanged("IsMgrCountryNameUkrChanged"); } }</v>
+        <v>public bool IsMgrPositionChanged { get { return _IsMgrPositionChanged; } set { _IsMgrPositionChanged = value; OnPropertyChanged("IsMgrPositionChanged"); } }</v>
       </c>
     </row>
     <row r="92" spans="7:12" x14ac:dyDescent="0.25">
@@ -13862,19 +14084,19 @@
         <v>460</v>
       </c>
       <c r="I92" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J92" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrCountryNameUkrNew</v>
+        <v>_MgrPositionNew</v>
       </c>
       <c r="K92" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrCountryNameUkrNew;</v>
+        <v>private string _MgrPositionNew;</v>
       </c>
       <c r="L92" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrCountryNameUkrNew { get { return _MgrCountryNameUkrNew; } set { _MgrCountryNameUkrNew = value; OnPropertyChanged("MgrCountryNameUkrNew"); } }</v>
+        <v>public string MgrPositionNew { get { return _MgrPositionNew; } set { _MgrPositionNew = value; OnPropertyChanged("MgrPositionNew"); } }</v>
       </c>
     </row>
     <row r="93" spans="7:12" x14ac:dyDescent="0.25">
@@ -13885,19 +14107,19 @@
         <v>460</v>
       </c>
       <c r="I93" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J93" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrCountryNameUkrOld</v>
+        <v>_MgrPositionOld</v>
       </c>
       <c r="K93" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrCountryNameUkrOld;</v>
+        <v>private string _MgrPositionOld;</v>
       </c>
       <c r="L93" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrCountryNameUkrOld { get { return _MgrCountryNameUkrOld; } set { _MgrCountryNameUkrOld = value; OnPropertyChanged("MgrCountryNameUkrOld"); } }</v>
+        <v>public string MgrPositionOld { get { return _MgrPositionOld; } set { _MgrPositionOld = value; OnPropertyChanged("MgrPositionOld"); } }</v>
       </c>
     </row>
     <row r="94" spans="7:12" x14ac:dyDescent="0.25">
@@ -13908,19 +14130,19 @@
         <v>566</v>
       </c>
       <c r="I94" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="J94" t="str">
         <f t="shared" si="24"/>
-        <v>_IsMgrSurnameChanged</v>
+        <v>_IsMgrCountryISO3CodeChanged</v>
       </c>
       <c r="K94" t="str">
         <f t="shared" si="25"/>
-        <v>private bool _IsMgrSurnameChanged;</v>
+        <v>private bool _IsMgrCountryISO3CodeChanged;</v>
       </c>
       <c r="L94" t="str">
         <f t="shared" si="26"/>
-        <v>public bool IsMgrSurnameChanged { get { return _IsMgrSurnameChanged; } set { _IsMgrSurnameChanged = value; OnPropertyChanged("IsMgrSurnameChanged"); } }</v>
+        <v>public bool IsMgrCountryISO3CodeChanged { get { return _IsMgrCountryISO3CodeChanged; } set { _IsMgrCountryISO3CodeChanged = value; OnPropertyChanged("IsMgrCountryISO3CodeChanged"); } }</v>
       </c>
     </row>
     <row r="95" spans="7:12" x14ac:dyDescent="0.25">
@@ -13931,19 +14153,19 @@
         <v>460</v>
       </c>
       <c r="I95" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="J95" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrSurnameNew</v>
+        <v>_MgrCountryISO3CodeNew</v>
       </c>
       <c r="K95" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrSurnameNew;</v>
+        <v>private string _MgrCountryISO3CodeNew;</v>
       </c>
       <c r="L95" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrSurnameNew { get { return _MgrSurnameNew; } set { _MgrSurnameNew = value; OnPropertyChanged("MgrSurnameNew"); } }</v>
+        <v>public string MgrCountryISO3CodeNew { get { return _MgrCountryISO3CodeNew; } set { _MgrCountryISO3CodeNew = value; OnPropertyChanged("MgrCountryISO3CodeNew"); } }</v>
       </c>
     </row>
     <row r="96" spans="7:12" x14ac:dyDescent="0.25">
@@ -13954,19 +14176,19 @@
         <v>460</v>
       </c>
       <c r="I96" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="J96" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrSurnameOld</v>
+        <v>_MgrCountryISO3CodeOld</v>
       </c>
       <c r="K96" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrSurnameOld;</v>
+        <v>private string _MgrCountryISO3CodeOld;</v>
       </c>
       <c r="L96" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrSurnameOld { get { return _MgrSurnameOld; } set { _MgrSurnameOld = value; OnPropertyChanged("MgrSurnameOld"); } }</v>
+        <v>public string MgrCountryISO3CodeOld { get { return _MgrCountryISO3CodeOld; } set { _MgrCountryISO3CodeOld = value; OnPropertyChanged("MgrCountryISO3CodeOld"); } }</v>
       </c>
     </row>
     <row r="97" spans="7:12" x14ac:dyDescent="0.25">
@@ -13977,19 +14199,19 @@
         <v>566</v>
       </c>
       <c r="I97" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="J97" t="str">
         <f t="shared" si="24"/>
-        <v>_IsMgrNameChanged</v>
+        <v>_IsMgrCountryNameUkrChanged</v>
       </c>
       <c r="K97" t="str">
         <f t="shared" si="25"/>
-        <v>private bool _IsMgrNameChanged;</v>
+        <v>private bool _IsMgrCountryNameUkrChanged;</v>
       </c>
       <c r="L97" t="str">
         <f t="shared" si="26"/>
-        <v>public bool IsMgrNameChanged { get { return _IsMgrNameChanged; } set { _IsMgrNameChanged = value; OnPropertyChanged("IsMgrNameChanged"); } }</v>
+        <v>public bool IsMgrCountryNameUkrChanged { get { return _IsMgrCountryNameUkrChanged; } set { _IsMgrCountryNameUkrChanged = value; OnPropertyChanged("IsMgrCountryNameUkrChanged"); } }</v>
       </c>
     </row>
     <row r="98" spans="7:12" x14ac:dyDescent="0.25">
@@ -14000,19 +14222,19 @@
         <v>460</v>
       </c>
       <c r="I98" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="J98" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrNameNew</v>
+        <v>_MgrCountryNameUkrNew</v>
       </c>
       <c r="K98" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrNameNew;</v>
+        <v>private string _MgrCountryNameUkrNew;</v>
       </c>
       <c r="L98" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrNameNew { get { return _MgrNameNew; } set { _MgrNameNew = value; OnPropertyChanged("MgrNameNew"); } }</v>
+        <v>public string MgrCountryNameUkrNew { get { return _MgrCountryNameUkrNew; } set { _MgrCountryNameUkrNew = value; OnPropertyChanged("MgrCountryNameUkrNew"); } }</v>
       </c>
     </row>
     <row r="99" spans="7:12" x14ac:dyDescent="0.25">
@@ -14023,19 +14245,19 @@
         <v>460</v>
       </c>
       <c r="I99" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="J99" t="str">
         <f t="shared" si="24"/>
-        <v>_MgrNameOld</v>
+        <v>_MgrCountryNameUkrOld</v>
       </c>
       <c r="K99" t="str">
         <f t="shared" si="25"/>
-        <v>private string _MgrNameOld;</v>
+        <v>private string _MgrCountryNameUkrOld;</v>
       </c>
       <c r="L99" t="str">
         <f t="shared" si="26"/>
-        <v>public string MgrNameOld { get { return _MgrNameOld; } set { _MgrNameOld = value; OnPropertyChanged("MgrNameOld"); } }</v>
+        <v>public string MgrCountryNameUkrOld { get { return _MgrCountryNameUkrOld; } set { _MgrCountryNameUkrOld = value; OnPropertyChanged("MgrCountryNameUkrOld"); } }</v>
       </c>
     </row>
     <row r="100" spans="7:12" x14ac:dyDescent="0.25">
@@ -14046,19 +14268,19 @@
         <v>566</v>
       </c>
       <c r="I100" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="J100" t="str">
         <f t="shared" si="24"/>
-        <v>_IsMgrMiddleNameChanged</v>
+        <v>_IsMgrSurnameChanged</v>
       </c>
       <c r="K100" t="str">
         <f t="shared" si="25"/>
-        <v>private bool _IsMgrMiddleNameChanged;</v>
+        <v>private bool _IsMgrSurnameChanged;</v>
       </c>
       <c r="L100" t="str">
         <f t="shared" si="26"/>
-        <v>public bool IsMgrMiddleNameChanged { get { return _IsMgrMiddleNameChanged; } set { _IsMgrMiddleNameChanged = value; OnPropertyChanged("IsMgrMiddleNameChanged"); } }</v>
+        <v>public bool IsMgrSurnameChanged { get { return _IsMgrSurnameChanged; } set { _IsMgrSurnameChanged = value; OnPropertyChanged("IsMgrSurnameChanged"); } }</v>
       </c>
     </row>
     <row r="101" spans="7:12" x14ac:dyDescent="0.25">
@@ -14069,19 +14291,19 @@
         <v>460</v>
       </c>
       <c r="I101" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="J101" t="str">
-        <f t="shared" ref="J101:J114" si="30">"_"&amp;I101</f>
-        <v>_MgrMiddleNameNew</v>
+        <f t="shared" si="24"/>
+        <v>_MgrSurnameNew</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" ref="K101:K114" si="31">"private " &amp; H101 &amp; " " &amp; J101 &amp; ";"</f>
-        <v>private string _MgrMiddleNameNew;</v>
+        <f t="shared" si="25"/>
+        <v>private string _MgrSurnameNew;</v>
       </c>
       <c r="L101" t="str">
-        <f t="shared" ref="L101:L114" si="32">G101&amp; " " &amp;H101&amp; " " &amp;I101 &amp; " { get { return " &amp; J101 &amp; "; } set { " &amp;J101 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I101 &amp; CHAR(34) &amp; "); } }"</f>
-        <v>public string MgrMiddleNameNew { get { return _MgrMiddleNameNew; } set { _MgrMiddleNameNew = value; OnPropertyChanged("MgrMiddleNameNew"); } }</v>
+        <f t="shared" si="26"/>
+        <v>public string MgrSurnameNew { get { return _MgrSurnameNew; } set { _MgrSurnameNew = value; OnPropertyChanged("MgrSurnameNew"); } }</v>
       </c>
     </row>
     <row r="102" spans="7:12" x14ac:dyDescent="0.25">
@@ -14092,19 +14314,19 @@
         <v>460</v>
       </c>
       <c r="I102" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="J102" t="str">
-        <f t="shared" si="30"/>
-        <v>_MgrMiddleNameOld</v>
+        <f t="shared" si="24"/>
+        <v>_MgrSurnameOld</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="31"/>
-        <v>private string _MgrMiddleNameOld;</v>
+        <f t="shared" si="25"/>
+        <v>private string _MgrSurnameOld;</v>
       </c>
       <c r="L102" t="str">
-        <f t="shared" si="32"/>
-        <v>public string MgrMiddleNameOld { get { return _MgrMiddleNameOld; } set { _MgrMiddleNameOld = value; OnPropertyChanged("MgrMiddleNameOld"); } }</v>
+        <f t="shared" si="26"/>
+        <v>public string MgrSurnameOld { get { return _MgrSurnameOld; } set { _MgrSurnameOld = value; OnPropertyChanged("MgrSurnameOld"); } }</v>
       </c>
     </row>
     <row r="103" spans="7:12" x14ac:dyDescent="0.25">
@@ -14115,19 +14337,19 @@
         <v>566</v>
       </c>
       <c r="I103" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="J103" t="str">
-        <f t="shared" si="30"/>
-        <v>_IsMgrSurnameAtBirthChanged</v>
+        <f t="shared" si="24"/>
+        <v>_IsMgrNameChanged</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="31"/>
-        <v>private bool _IsMgrSurnameAtBirthChanged;</v>
+        <f t="shared" si="25"/>
+        <v>private bool _IsMgrNameChanged;</v>
       </c>
       <c r="L103" t="str">
-        <f t="shared" si="32"/>
-        <v>public bool IsMgrSurnameAtBirthChanged { get { return _IsMgrSurnameAtBirthChanged; } set { _IsMgrSurnameAtBirthChanged = value; OnPropertyChanged("IsMgrSurnameAtBirthChanged"); } }</v>
+        <f t="shared" si="26"/>
+        <v>public bool IsMgrNameChanged { get { return _IsMgrNameChanged; } set { _IsMgrNameChanged = value; OnPropertyChanged("IsMgrNameChanged"); } }</v>
       </c>
     </row>
     <row r="104" spans="7:12" x14ac:dyDescent="0.25">
@@ -14138,19 +14360,19 @@
         <v>460</v>
       </c>
       <c r="I104" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="J104" t="str">
-        <f t="shared" si="30"/>
-        <v>_MgrSurnameAtBirthNew</v>
+        <f t="shared" si="24"/>
+        <v>_MgrNameNew</v>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="31"/>
-        <v>private string _MgrSurnameAtBirthNew;</v>
+        <f t="shared" si="25"/>
+        <v>private string _MgrNameNew;</v>
       </c>
       <c r="L104" t="str">
-        <f t="shared" si="32"/>
-        <v>public string MgrSurnameAtBirthNew { get { return _MgrSurnameAtBirthNew; } set { _MgrSurnameAtBirthNew = value; OnPropertyChanged("MgrSurnameAtBirthNew"); } }</v>
+        <f t="shared" si="26"/>
+        <v>public string MgrNameNew { get { return _MgrNameNew; } set { _MgrNameNew = value; OnPropertyChanged("MgrNameNew"); } }</v>
       </c>
     </row>
     <row r="105" spans="7:12" x14ac:dyDescent="0.25">
@@ -14161,19 +14383,19 @@
         <v>460</v>
       </c>
       <c r="I105" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="J105" t="str">
-        <f t="shared" si="30"/>
-        <v>_MgrSurnameAtBirthOld</v>
+        <f t="shared" si="24"/>
+        <v>_MgrNameOld</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="31"/>
-        <v>private string _MgrSurnameAtBirthOld;</v>
+        <f t="shared" si="25"/>
+        <v>private string _MgrNameOld;</v>
       </c>
       <c r="L105" t="str">
-        <f t="shared" si="32"/>
-        <v>public string MgrSurnameAtBirthOld { get { return _MgrSurnameAtBirthOld; } set { _MgrSurnameAtBirthOld = value; OnPropertyChanged("MgrSurnameAtBirthOld"); } }</v>
+        <f t="shared" si="26"/>
+        <v>public string MgrNameOld { get { return _MgrNameOld; } set { _MgrNameOld = value; OnPropertyChanged("MgrNameOld"); } }</v>
       </c>
     </row>
     <row r="106" spans="7:12" x14ac:dyDescent="0.25">
@@ -14184,19 +14406,19 @@
         <v>566</v>
       </c>
       <c r="I106" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="J106" t="str">
-        <f t="shared" si="30"/>
-        <v>_IsMgrTaxOrSocSecIDChanged</v>
+        <f t="shared" si="24"/>
+        <v>_IsMgrMiddleNameChanged</v>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="31"/>
-        <v>private bool _IsMgrTaxOrSocSecIDChanged;</v>
+        <f t="shared" si="25"/>
+        <v>private bool _IsMgrMiddleNameChanged;</v>
       </c>
       <c r="L106" t="str">
-        <f t="shared" si="32"/>
-        <v>public bool IsMgrTaxOrSocSecIDChanged { get { return _IsMgrTaxOrSocSecIDChanged; } set { _IsMgrTaxOrSocSecIDChanged = value; OnPropertyChanged("IsMgrTaxOrSocSecIDChanged"); } }</v>
+        <f t="shared" si="26"/>
+        <v>public bool IsMgrMiddleNameChanged { get { return _IsMgrMiddleNameChanged; } set { _IsMgrMiddleNameChanged = value; OnPropertyChanged("IsMgrMiddleNameChanged"); } }</v>
       </c>
     </row>
     <row r="107" spans="7:12" x14ac:dyDescent="0.25">
@@ -14207,19 +14429,19 @@
         <v>460</v>
       </c>
       <c r="I107" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="J107" t="str">
-        <f t="shared" si="30"/>
-        <v>_MgrTaxOrSocSecIDNew</v>
+        <f t="shared" ref="J107:J120" si="36">"_"&amp;I107</f>
+        <v>_MgrMiddleNameNew</v>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="31"/>
-        <v>private string _MgrTaxOrSocSecIDNew;</v>
+        <f t="shared" ref="K107:K120" si="37">"private " &amp; H107 &amp; " " &amp; J107 &amp; ";"</f>
+        <v>private string _MgrMiddleNameNew;</v>
       </c>
       <c r="L107" t="str">
-        <f t="shared" si="32"/>
-        <v>public string MgrTaxOrSocSecIDNew { get { return _MgrTaxOrSocSecIDNew; } set { _MgrTaxOrSocSecIDNew = value; OnPropertyChanged("MgrTaxOrSocSecIDNew"); } }</v>
+        <f t="shared" ref="L107:L120" si="38">G107&amp; " " &amp;H107&amp; " " &amp;I107 &amp; " { get { return " &amp; J107 &amp; "; } set { " &amp;J107 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I107 &amp; CHAR(34) &amp; "); } }"</f>
+        <v>public string MgrMiddleNameNew { get { return _MgrMiddleNameNew; } set { _MgrMiddleNameNew = value; OnPropertyChanged("MgrMiddleNameNew"); } }</v>
       </c>
     </row>
     <row r="108" spans="7:12" x14ac:dyDescent="0.25">
@@ -14230,19 +14452,19 @@
         <v>460</v>
       </c>
       <c r="I108" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="J108" t="str">
-        <f t="shared" si="30"/>
-        <v>_MgrTaxOrSocSecIDOld</v>
+        <f t="shared" si="36"/>
+        <v>_MgrMiddleNameOld</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="31"/>
-        <v>private string _MgrTaxOrSocSecIDOld;</v>
+        <f t="shared" si="37"/>
+        <v>private string _MgrMiddleNameOld;</v>
       </c>
       <c r="L108" t="str">
-        <f t="shared" si="32"/>
-        <v>public string MgrTaxOrSocSecIDOld { get { return _MgrTaxOrSocSecIDOld; } set { _MgrTaxOrSocSecIDOld = value; OnPropertyChanged("MgrTaxOrSocSecIDOld"); } }</v>
+        <f t="shared" si="38"/>
+        <v>public string MgrMiddleNameOld { get { return _MgrMiddleNameOld; } set { _MgrMiddleNameOld = value; OnPropertyChanged("MgrMiddleNameOld"); } }</v>
       </c>
     </row>
     <row r="109" spans="7:12" x14ac:dyDescent="0.25">
@@ -14253,19 +14475,19 @@
         <v>566</v>
       </c>
       <c r="I109" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="J109" t="str">
-        <f t="shared" si="30"/>
-        <v>_IsMgrPassportIDChanged</v>
+        <f t="shared" si="36"/>
+        <v>_IsMgrSurnameAtBirthChanged</v>
       </c>
       <c r="K109" t="str">
-        <f t="shared" si="31"/>
-        <v>private bool _IsMgrPassportIDChanged;</v>
+        <f t="shared" si="37"/>
+        <v>private bool _IsMgrSurnameAtBirthChanged;</v>
       </c>
       <c r="L109" t="str">
-        <f t="shared" si="32"/>
-        <v>public bool IsMgrPassportIDChanged { get { return _IsMgrPassportIDChanged; } set { _IsMgrPassportIDChanged = value; OnPropertyChanged("IsMgrPassportIDChanged"); } }</v>
+        <f t="shared" si="38"/>
+        <v>public bool IsMgrSurnameAtBirthChanged { get { return _IsMgrSurnameAtBirthChanged; } set { _IsMgrSurnameAtBirthChanged = value; OnPropertyChanged("IsMgrSurnameAtBirthChanged"); } }</v>
       </c>
     </row>
     <row r="110" spans="7:12" x14ac:dyDescent="0.25">
@@ -14276,19 +14498,19 @@
         <v>460</v>
       </c>
       <c r="I110" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="J110" t="str">
-        <f t="shared" si="30"/>
-        <v>_MgrPassportIDNew</v>
+        <f t="shared" si="36"/>
+        <v>_MgrSurnameAtBirthNew</v>
       </c>
       <c r="K110" t="str">
-        <f t="shared" si="31"/>
-        <v>private string _MgrPassportIDNew;</v>
+        <f t="shared" si="37"/>
+        <v>private string _MgrSurnameAtBirthNew;</v>
       </c>
       <c r="L110" t="str">
-        <f t="shared" si="32"/>
-        <v>public string MgrPassportIDNew { get { return _MgrPassportIDNew; } set { _MgrPassportIDNew = value; OnPropertyChanged("MgrPassportIDNew"); } }</v>
+        <f t="shared" si="38"/>
+        <v>public string MgrSurnameAtBirthNew { get { return _MgrSurnameAtBirthNew; } set { _MgrSurnameAtBirthNew = value; OnPropertyChanged("MgrSurnameAtBirthNew"); } }</v>
       </c>
     </row>
     <row r="111" spans="7:12" x14ac:dyDescent="0.25">
@@ -14299,19 +14521,19 @@
         <v>460</v>
       </c>
       <c r="I111" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="J111" t="str">
-        <f t="shared" si="30"/>
-        <v>_MgrPassportIDOld</v>
+        <f t="shared" si="36"/>
+        <v>_MgrSurnameAtBirthOld</v>
       </c>
       <c r="K111" t="str">
-        <f t="shared" si="31"/>
-        <v>private string _MgrPassportIDOld;</v>
+        <f t="shared" si="37"/>
+        <v>private string _MgrSurnameAtBirthOld;</v>
       </c>
       <c r="L111" t="str">
-        <f t="shared" si="32"/>
-        <v>public string MgrPassportIDOld { get { return _MgrPassportIDOld; } set { _MgrPassportIDOld = value; OnPropertyChanged("MgrPassportIDOld"); } }</v>
+        <f t="shared" si="38"/>
+        <v>public string MgrSurnameAtBirthOld { get { return _MgrSurnameAtBirthOld; } set { _MgrSurnameAtBirthOld = value; OnPropertyChanged("MgrSurnameAtBirthOld"); } }</v>
       </c>
     </row>
     <row r="112" spans="7:12" x14ac:dyDescent="0.25">
@@ -14322,19 +14544,19 @@
         <v>566</v>
       </c>
       <c r="I112" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="J112" t="str">
-        <f t="shared" si="30"/>
-        <v>_IsMgrPassIssuedDateChanged</v>
+        <f t="shared" si="36"/>
+        <v>_IsMgrTaxOrSocSecIDChanged</v>
       </c>
       <c r="K112" t="str">
-        <f t="shared" si="31"/>
-        <v>private bool _IsMgrPassIssuedDateChanged;</v>
+        <f t="shared" si="37"/>
+        <v>private bool _IsMgrTaxOrSocSecIDChanged;</v>
       </c>
       <c r="L112" t="str">
-        <f t="shared" si="32"/>
-        <v>public bool IsMgrPassIssuedDateChanged { get { return _IsMgrPassIssuedDateChanged; } set { _IsMgrPassIssuedDateChanged = value; OnPropertyChanged("IsMgrPassIssuedDateChanged"); } }</v>
+        <f t="shared" si="38"/>
+        <v>public bool IsMgrTaxOrSocSecIDChanged { get { return _IsMgrTaxOrSocSecIDChanged; } set { _IsMgrTaxOrSocSecIDChanged = value; OnPropertyChanged("IsMgrTaxOrSocSecIDChanged"); } }</v>
       </c>
     </row>
     <row r="113" spans="7:12" x14ac:dyDescent="0.25">
@@ -14342,22 +14564,22 @@
         <v>567</v>
       </c>
       <c r="H113" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="I113" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="J113" t="str">
-        <f t="shared" si="30"/>
-        <v>_MgrPassIssuedDateNew</v>
+        <f t="shared" si="36"/>
+        <v>_MgrTaxOrSocSecIDNew</v>
       </c>
       <c r="K113" t="str">
-        <f t="shared" si="31"/>
-        <v>private DateTime? _MgrPassIssuedDateNew;</v>
+        <f t="shared" si="37"/>
+        <v>private string _MgrTaxOrSocSecIDNew;</v>
       </c>
       <c r="L113" t="str">
-        <f t="shared" si="32"/>
-        <v>public DateTime? MgrPassIssuedDateNew { get { return _MgrPassIssuedDateNew; } set { _MgrPassIssuedDateNew = value; OnPropertyChanged("MgrPassIssuedDateNew"); } }</v>
+        <f t="shared" si="38"/>
+        <v>public string MgrTaxOrSocSecIDNew { get { return _MgrTaxOrSocSecIDNew; } set { _MgrTaxOrSocSecIDNew = value; OnPropertyChanged("MgrTaxOrSocSecIDNew"); } }</v>
       </c>
     </row>
     <row r="114" spans="7:12" x14ac:dyDescent="0.25">
@@ -14365,22 +14587,298 @@
         <v>567</v>
       </c>
       <c r="H114" t="s">
+        <v>460</v>
+      </c>
+      <c r="I114" t="s">
+        <v>535</v>
+      </c>
+      <c r="J114" t="str">
+        <f t="shared" si="36"/>
+        <v>_MgrTaxOrSocSecIDOld</v>
+      </c>
+      <c r="K114" t="str">
+        <f t="shared" si="37"/>
+        <v>private string _MgrTaxOrSocSecIDOld;</v>
+      </c>
+      <c r="L114" t="str">
+        <f t="shared" si="38"/>
+        <v>public string MgrTaxOrSocSecIDOld { get { return _MgrTaxOrSocSecIDOld; } set { _MgrTaxOrSocSecIDOld = value; OnPropertyChanged("MgrTaxOrSocSecIDOld"); } }</v>
+      </c>
+    </row>
+    <row r="115" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G115" t="s">
+        <v>567</v>
+      </c>
+      <c r="H115" t="s">
+        <v>566</v>
+      </c>
+      <c r="I115" t="s">
+        <v>536</v>
+      </c>
+      <c r="J115" t="str">
+        <f t="shared" si="36"/>
+        <v>_IsMgrPassportIDChanged</v>
+      </c>
+      <c r="K115" t="str">
+        <f t="shared" si="37"/>
+        <v>private bool _IsMgrPassportIDChanged;</v>
+      </c>
+      <c r="L115" t="str">
+        <f t="shared" si="38"/>
+        <v>public bool IsMgrPassportIDChanged { get { return _IsMgrPassportIDChanged; } set { _IsMgrPassportIDChanged = value; OnPropertyChanged("IsMgrPassportIDChanged"); } }</v>
+      </c>
+    </row>
+    <row r="116" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G116" t="s">
+        <v>567</v>
+      </c>
+      <c r="H116" t="s">
+        <v>460</v>
+      </c>
+      <c r="I116" t="s">
+        <v>564</v>
+      </c>
+      <c r="J116" t="str">
+        <f t="shared" si="36"/>
+        <v>_MgrPassportIDNew</v>
+      </c>
+      <c r="K116" t="str">
+        <f t="shared" si="37"/>
+        <v>private string _MgrPassportIDNew;</v>
+      </c>
+      <c r="L116" t="str">
+        <f t="shared" si="38"/>
+        <v>public string MgrPassportIDNew { get { return _MgrPassportIDNew; } set { _MgrPassportIDNew = value; OnPropertyChanged("MgrPassportIDNew"); } }</v>
+      </c>
+    </row>
+    <row r="117" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G117" t="s">
+        <v>567</v>
+      </c>
+      <c r="H117" t="s">
+        <v>460</v>
+      </c>
+      <c r="I117" t="s">
+        <v>537</v>
+      </c>
+      <c r="J117" t="str">
+        <f t="shared" si="36"/>
+        <v>_MgrPassportIDOld</v>
+      </c>
+      <c r="K117" t="str">
+        <f t="shared" si="37"/>
+        <v>private string _MgrPassportIDOld;</v>
+      </c>
+      <c r="L117" t="str">
+        <f t="shared" si="38"/>
+        <v>public string MgrPassportIDOld { get { return _MgrPassportIDOld; } set { _MgrPassportIDOld = value; OnPropertyChanged("MgrPassportIDOld"); } }</v>
+      </c>
+    </row>
+    <row r="118" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G118" t="s">
+        <v>567</v>
+      </c>
+      <c r="H118" t="s">
+        <v>566</v>
+      </c>
+      <c r="I118" t="s">
+        <v>538</v>
+      </c>
+      <c r="J118" t="str">
+        <f t="shared" si="36"/>
+        <v>_IsMgrPassIssuedDateChanged</v>
+      </c>
+      <c r="K118" t="str">
+        <f t="shared" si="37"/>
+        <v>private bool _IsMgrPassIssuedDateChanged;</v>
+      </c>
+      <c r="L118" t="str">
+        <f t="shared" si="38"/>
+        <v>public bool IsMgrPassIssuedDateChanged { get { return _IsMgrPassIssuedDateChanged; } set { _IsMgrPassIssuedDateChanged = value; OnPropertyChanged("IsMgrPassIssuedDateChanged"); } }</v>
+      </c>
+    </row>
+    <row r="119" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G119" t="s">
+        <v>567</v>
+      </c>
+      <c r="H119" t="s">
         <v>486</v>
       </c>
-      <c r="I114" t="s">
+      <c r="I119" t="s">
+        <v>565</v>
+      </c>
+      <c r="J119" t="str">
+        <f t="shared" si="36"/>
+        <v>_MgrPassIssuedDateNew</v>
+      </c>
+      <c r="K119" t="str">
+        <f t="shared" si="37"/>
+        <v>private DateTime? _MgrPassIssuedDateNew;</v>
+      </c>
+      <c r="L119" t="str">
+        <f t="shared" si="38"/>
+        <v>public DateTime? MgrPassIssuedDateNew { get { return _MgrPassIssuedDateNew; } set { _MgrPassIssuedDateNew = value; OnPropertyChanged("MgrPassIssuedDateNew"); } }</v>
+      </c>
+    </row>
+    <row r="120" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G120" t="s">
+        <v>567</v>
+      </c>
+      <c r="H120" t="s">
+        <v>486</v>
+      </c>
+      <c r="I120" t="s">
         <v>539</v>
       </c>
-      <c r="J114" t="str">
-        <f t="shared" si="30"/>
+      <c r="J120" t="str">
+        <f t="shared" si="36"/>
         <v>_MgrPassIssuedDateOld</v>
       </c>
-      <c r="K114" t="str">
-        <f t="shared" si="31"/>
+      <c r="K120" t="str">
+        <f t="shared" si="37"/>
         <v>private DateTime? _MgrPassIssuedDateOld;</v>
       </c>
-      <c r="L114" t="str">
-        <f t="shared" si="32"/>
+      <c r="L120" t="str">
+        <f t="shared" si="38"/>
         <v>public DateTime? MgrPassIssuedDateOld { get { return _MgrPassIssuedDateOld; } set { _MgrPassIssuedDateOld = value; OnPropertyChanged("MgrPassIssuedDateOld"); } }</v>
+      </c>
+    </row>
+    <row r="121" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G121" t="s">
+        <v>567</v>
+      </c>
+      <c r="H121" t="s">
+        <v>566</v>
+      </c>
+      <c r="I121" t="s">
+        <v>603</v>
+      </c>
+      <c r="J121" t="str">
+        <f t="shared" ref="J121:J123" si="39">"_"&amp;I121</f>
+        <v>_IsOperationsListingChanged</v>
+      </c>
+      <c r="K121" t="str">
+        <f t="shared" ref="K121:K123" si="40">"private " &amp; H121 &amp; " " &amp; J121 &amp; ";"</f>
+        <v>private bool _IsOperationsListingChanged;</v>
+      </c>
+      <c r="L121" t="str">
+        <f t="shared" ref="L121:L123" si="41">G121&amp; " " &amp;H121&amp; " " &amp;I121 &amp; " { get { return " &amp; J121 &amp; "; } set { " &amp;J121 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I121 &amp; CHAR(34) &amp; "); } }"</f>
+        <v>public bool IsOperationsListingChanged { get { return _IsOperationsListingChanged; } set { _IsOperationsListingChanged = value; OnPropertyChanged("IsOperationsListingChanged"); } }</v>
+      </c>
+    </row>
+    <row r="122" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G122" t="s">
+        <v>567</v>
+      </c>
+      <c r="H122" t="s">
+        <v>460</v>
+      </c>
+      <c r="I122" t="s">
+        <v>604</v>
+      </c>
+      <c r="J122" t="str">
+        <f t="shared" si="39"/>
+        <v>_OperationsListingNew</v>
+      </c>
+      <c r="K122" t="str">
+        <f t="shared" si="40"/>
+        <v>private string _OperationsListingNew;</v>
+      </c>
+      <c r="L122" t="str">
+        <f t="shared" si="41"/>
+        <v>public string OperationsListingNew { get { return _OperationsListingNew; } set { _OperationsListingNew = value; OnPropertyChanged("OperationsListingNew"); } }</v>
+      </c>
+    </row>
+    <row r="123" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G123" t="s">
+        <v>567</v>
+      </c>
+      <c r="H123" t="s">
+        <v>460</v>
+      </c>
+      <c r="I123" t="s">
+        <v>605</v>
+      </c>
+      <c r="J123" t="str">
+        <f t="shared" si="39"/>
+        <v>_OperationsListingOld</v>
+      </c>
+      <c r="K123" t="str">
+        <f t="shared" si="40"/>
+        <v>private string _OperationsListingOld;</v>
+      </c>
+      <c r="L123" t="str">
+        <f t="shared" si="41"/>
+        <v>public string OperationsListingOld { get { return _OperationsListingOld; } set { _OperationsListingOld = value; OnPropertyChanged("OperationsListingOld"); } }</v>
+      </c>
+    </row>
+    <row r="124" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G124" t="s">
+        <v>567</v>
+      </c>
+      <c r="H124" t="s">
+        <v>566</v>
+      </c>
+      <c r="I124" t="s">
+        <v>607</v>
+      </c>
+      <c r="J124" t="str">
+        <f t="shared" ref="J124:J126" si="42">"_"&amp;I124</f>
+        <v>_IsStatusChanged</v>
+      </c>
+      <c r="K124" t="str">
+        <f t="shared" ref="K124:K126" si="43">"private " &amp; H124 &amp; " " &amp; J124 &amp; ";"</f>
+        <v>private bool _IsStatusChanged;</v>
+      </c>
+      <c r="L124" t="str">
+        <f t="shared" ref="L124:L126" si="44">G124&amp; " " &amp;H124&amp; " " &amp;I124 &amp; " { get { return " &amp; J124 &amp; "; } set { " &amp;J124 &amp; " = value; OnPropertyChanged(" &amp; CHAR(34) &amp; I124 &amp; CHAR(34) &amp; "); } }"</f>
+        <v>public bool IsStatusChanged { get { return _IsStatusChanged; } set { _IsStatusChanged = value; OnPropertyChanged("IsStatusChanged"); } }</v>
+      </c>
+    </row>
+    <row r="125" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G125" t="s">
+        <v>567</v>
+      </c>
+      <c r="H125" t="s">
+        <v>313</v>
+      </c>
+      <c r="I125" t="s">
+        <v>608</v>
+      </c>
+      <c r="J125" t="str">
+        <f t="shared" si="42"/>
+        <v>_StatusNew</v>
+      </c>
+      <c r="K125" t="str">
+        <f t="shared" si="43"/>
+        <v>private BankBranchStatusType _StatusNew;</v>
+      </c>
+      <c r="L125" t="str">
+        <f t="shared" si="44"/>
+        <v>public BankBranchStatusType StatusNew { get { return _StatusNew; } set { _StatusNew = value; OnPropertyChanged("StatusNew"); } }</v>
+      </c>
+    </row>
+    <row r="126" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G126" t="s">
+        <v>567</v>
+      </c>
+      <c r="H126" t="s">
+        <v>313</v>
+      </c>
+      <c r="I126" t="s">
+        <v>609</v>
+      </c>
+      <c r="J126" t="str">
+        <f t="shared" si="42"/>
+        <v>_StatusOld</v>
+      </c>
+      <c r="K126" t="str">
+        <f t="shared" si="43"/>
+        <v>private BankBranchStatusType _StatusOld;</v>
+      </c>
+      <c r="L126" t="str">
+        <f t="shared" si="44"/>
+        <v>public BankBranchStatusType StatusOld { get { return _StatusOld; } set { _StatusOld = value; OnPropertyChanged("StatusOld"); } }</v>
       </c>
     </row>
   </sheetData>
@@ -14394,7 +14892,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>